<commit_message>
Speed Master N3 Vocab.xlsx  ->  Myanmar Spelling updated
</commit_message>
<xml_diff>
--- a/preparing/Speed Master N3 Vocab.xlsx
+++ b/preparing/Speed Master N3 Vocab.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6628" uniqueCount="5965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6630" uniqueCount="5966">
   <si>
     <t>yesterday</t>
   </si>
@@ -16366,9 +16366,6 @@
   </si>
   <si>
     <t>ေတာင္းဆိုျခင္း</t>
-  </si>
-  <si>
-    <t>ေတာင္ဆိုသည္</t>
   </si>
   <si>
     <t>မွီခိုအားထားသည္</t>
@@ -17137,9 +17134,6 @@
     <t>တောင်းဆိုခြင်း</t>
   </si>
   <si>
-    <t>တောင်ဆိုသည်</t>
-  </si>
-  <si>
     <t>မှီခိုအားထားသည်</t>
   </si>
   <si>
@@ -17913,6 +17907,16 @@
   <si>
     <t>Part1 : 8,9,10,11,12
 Myanmar Definition (#Zawgyi) added.</t>
+  </si>
+  <si>
+    <t>ေတာင္းဆိုသည္</t>
+  </si>
+  <si>
+    <t>တောင်းဆိုသည်</t>
+  </si>
+  <si>
+    <t>Part1 : 4
+Myanmar Definition missing spelling updated</t>
   </si>
 </sst>
 </file>
@@ -18312,7 +18316,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18331,7 +18335,7 @@
         <v>5426</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>5481</v>
+        <v>5480</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>5425</v>
@@ -18342,13 +18346,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5482</v>
+        <v>5481</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>5482</v>
+        <v>5481</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>5482</v>
+        <v>5481</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -18359,10 +18363,10 @@
         <v>43367</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>5483</v>
+        <v>5482</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>5579</v>
+        <v>5578</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -18373,17 +18377,25 @@
         <v>43389</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5483</v>
+        <v>5482</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>5964</v>
+        <v>5962</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43392</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5482</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>5965</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
@@ -18431,8 +18443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1533"/>
   <sheetViews>
-    <sheetView topLeftCell="A401" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F427" sqref="F427"/>
+    <sheetView topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="19.8" x14ac:dyDescent="0.6"/>
@@ -18479,7 +18491,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>5580</v>
+        <v>5579</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3868</v>
@@ -18496,7 +18508,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>5581</v>
+        <v>5580</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>3869</v>
@@ -18513,7 +18525,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>5582</v>
+        <v>5581</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>3870</v>
@@ -18530,7 +18542,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>5583</v>
+        <v>5582</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>3871</v>
@@ -18547,10 +18559,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>5817</v>
+        <v>5815</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5818</v>
+        <v>5816</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.6">
@@ -18564,10 +18576,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>5820</v>
+        <v>5818</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>5819</v>
+        <v>5817</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.6">
@@ -18581,7 +18593,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>5584</v>
+        <v>5583</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>3872</v>
@@ -18598,7 +18610,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>5585</v>
+        <v>5584</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>3873</v>
@@ -18615,7 +18627,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>5586</v>
+        <v>5585</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>3874</v>
@@ -18632,7 +18644,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>5587</v>
+        <v>5586</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>3875</v>
@@ -18649,7 +18661,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>5588</v>
+        <v>5587</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>3876</v>
@@ -18666,7 +18678,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>5589</v>
+        <v>5588</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>3877</v>
@@ -18683,7 +18695,7 @@
         <v>24</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>5590</v>
+        <v>5589</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>3878</v>
@@ -18700,7 +18712,7 @@
         <v>26</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>5591</v>
+        <v>5590</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>3879</v>
@@ -18717,7 +18729,7 @@
         <v>28</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>5592</v>
+        <v>5591</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>3880</v>
@@ -18734,7 +18746,7 @@
         <v>30</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>5593</v>
+        <v>5592</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>3881</v>
@@ -18751,7 +18763,7 @@
         <v>32</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>5594</v>
+        <v>5593</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>3882</v>
@@ -18768,7 +18780,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>5595</v>
+        <v>5594</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>3883</v>
@@ -18785,7 +18797,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>5596</v>
+        <v>5595</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>3884</v>
@@ -18802,7 +18814,7 @@
         <v>38</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>5597</v>
+        <v>5596</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>3887</v>
@@ -18819,7 +18831,7 @@
         <v>40</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>5598</v>
+        <v>5597</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>3888</v>
@@ -18836,7 +18848,7 @@
         <v>42</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>5599</v>
+        <v>5598</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>3885</v>
@@ -18853,7 +18865,7 @@
         <v>44</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>5600</v>
+        <v>5599</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>3886</v>
@@ -18870,7 +18882,7 @@
         <v>46</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>5601</v>
+        <v>5600</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>3889</v>
@@ -18887,7 +18899,7 @@
         <v>48</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>5602</v>
+        <v>5601</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>3890</v>
@@ -18904,7 +18916,7 @@
         <v>50</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>5603</v>
+        <v>5602</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>3891</v>
@@ -18921,7 +18933,7 @@
         <v>52</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>5604</v>
+        <v>5603</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>3892</v>
@@ -18938,7 +18950,7 @@
         <v>54</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>5605</v>
+        <v>5604</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>3893</v>
@@ -18955,7 +18967,7 @@
         <v>56</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>5606</v>
+        <v>5605</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>3894</v>
@@ -18989,7 +19001,7 @@
         <v>60</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>5607</v>
+        <v>5606</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>3896</v>
@@ -19023,7 +19035,7 @@
         <v>64</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>5608</v>
+        <v>5607</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>3898</v>
@@ -19040,7 +19052,7 @@
         <v>66</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>5609</v>
+        <v>5608</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>3899</v>
@@ -19057,7 +19069,7 @@
         <v>68</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>5610</v>
+        <v>5609</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>3900</v>
@@ -19074,7 +19086,7 @@
         <v>70</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>5611</v>
+        <v>5610</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>3901</v>
@@ -19091,7 +19103,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>5612</v>
+        <v>5611</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>3902</v>
@@ -19125,7 +19137,7 @@
         <v>76</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>5591</v>
+        <v>5590</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>3879</v>
@@ -19159,7 +19171,7 @@
         <v>80</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>5613</v>
+        <v>5612</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>3905</v>
@@ -19176,7 +19188,7 @@
         <v>82</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>5614</v>
+        <v>5613</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>3906</v>
@@ -19193,7 +19205,7 @@
         <v>84</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>5615</v>
+        <v>5614</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>3907</v>
@@ -19210,7 +19222,7 @@
         <v>86</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>5616</v>
+        <v>5615</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>3908</v>
@@ -19227,7 +19239,7 @@
         <v>88</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>5617</v>
+        <v>5616</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>3909</v>
@@ -19244,7 +19256,7 @@
         <v>90</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>5618</v>
+        <v>5617</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>3910</v>
@@ -19261,7 +19273,7 @@
         <v>92</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>5618</v>
+        <v>5617</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>3910</v>
@@ -19278,7 +19290,7 @@
         <v>94</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>5619</v>
+        <v>5618</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>3911</v>
@@ -19295,7 +19307,7 @@
         <v>96</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>5620</v>
+        <v>5619</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>3912</v>
@@ -19312,7 +19324,7 @@
         <v>98</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>5621</v>
+        <v>5620</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>3913</v>
@@ -19329,7 +19341,7 @@
         <v>100</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>5622</v>
+        <v>5621</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>3914</v>
@@ -19346,7 +19358,7 @@
         <v>102</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>5623</v>
+        <v>5622</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>3915</v>
@@ -19363,7 +19375,7 @@
         <v>104</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>5624</v>
+        <v>5623</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>3916</v>
@@ -19397,7 +19409,7 @@
         <v>108</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>5625</v>
+        <v>5624</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>3918</v>
@@ -19414,7 +19426,7 @@
         <v>110</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>5626</v>
+        <v>5625</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>3919</v>
@@ -19431,7 +19443,7 @@
         <v>112</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>5627</v>
+        <v>5626</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>3920</v>
@@ -19448,7 +19460,7 @@
         <v>114</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>5628</v>
+        <v>5627</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>3921</v>
@@ -19465,7 +19477,7 @@
         <v>116</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>5629</v>
+        <v>5628</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>3922</v>
@@ -19482,7 +19494,7 @@
         <v>118</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>5630</v>
+        <v>5629</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>3923</v>
@@ -19499,7 +19511,7 @@
         <v>120</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>5631</v>
+        <v>5630</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>3925</v>
@@ -19516,7 +19528,7 @@
         <v>122</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>5632</v>
+        <v>5631</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>3924</v>
@@ -19533,7 +19545,7 @@
         <v>124</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>5633</v>
+        <v>5632</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>3926</v>
@@ -19550,7 +19562,7 @@
         <v>126</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>5634</v>
+        <v>5633</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>3927</v>
@@ -19573,7 +19585,7 @@
         <v>186</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>5635</v>
+        <v>5634</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>5366</v>
@@ -19590,7 +19602,7 @@
         <v>188</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>5636</v>
+        <v>5635</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>5367</v>
@@ -19607,7 +19619,7 @@
         <v>190</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>5637</v>
+        <v>5636</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>5369</v>
@@ -19624,7 +19636,7 @@
         <v>192</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>5638</v>
+        <v>5637</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>5368</v>
@@ -19641,7 +19653,7 @@
         <v>194</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>5639</v>
+        <v>5638</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>5370</v>
@@ -19692,7 +19704,7 @@
         <v>200</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>5640</v>
+        <v>5639</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>5373</v>
@@ -19726,7 +19738,7 @@
         <v>204</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>5641</v>
+        <v>5640</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>5375</v>
@@ -19777,7 +19789,7 @@
         <v>210</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>5642</v>
+        <v>5641</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>5378</v>
@@ -19794,7 +19806,7 @@
         <v>212</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>5643</v>
+        <v>5642</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>5379</v>
@@ -19811,7 +19823,7 @@
         <v>214</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>5644</v>
+        <v>5643</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>5380</v>
@@ -19828,7 +19840,7 @@
         <v>216</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>5645</v>
+        <v>5644</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>5381</v>
@@ -19851,7 +19863,7 @@
         <v>233</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>5646</v>
+        <v>5645</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>5382</v>
@@ -19868,7 +19880,7 @@
         <v>235</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>5647</v>
+        <v>5646</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>5386</v>
@@ -19885,7 +19897,7 @@
         <v>237</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>5648</v>
+        <v>5647</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>5384</v>
@@ -19919,7 +19931,7 @@
         <v>241</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>5649</v>
+        <v>5648</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>5383</v>
@@ -19936,7 +19948,7 @@
         <v>243</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>5650</v>
+        <v>5649</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>5387</v>
@@ -19953,7 +19965,7 @@
         <v>245</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>5651</v>
+        <v>5650</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>5388</v>
@@ -19970,7 +19982,7 @@
         <v>247</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>5652</v>
+        <v>5651</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>5389</v>
@@ -19987,7 +19999,7 @@
         <v>249</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>5653</v>
+        <v>5652</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>5390</v>
@@ -20004,7 +20016,7 @@
         <v>251</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>5654</v>
+        <v>5653</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>5391</v>
@@ -20021,7 +20033,7 @@
         <v>253</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>5655</v>
+        <v>5654</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>5392</v>
@@ -20038,7 +20050,7 @@
         <v>255</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>5656</v>
+        <v>5655</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>5393</v>
@@ -20055,7 +20067,7 @@
         <v>257</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>5657</v>
+        <v>5656</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>5394</v>
@@ -20072,7 +20084,7 @@
         <v>259</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>5658</v>
+        <v>5657</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>5395</v>
@@ -20089,7 +20101,7 @@
         <v>261</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>5659</v>
+        <v>5658</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>5396</v>
@@ -20106,7 +20118,7 @@
         <v>263</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>5660</v>
+        <v>5659</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>5397</v>
@@ -20123,7 +20135,7 @@
         <v>265</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>5661</v>
+        <v>5660</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>5398</v>
@@ -20140,7 +20152,7 @@
         <v>267</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>5662</v>
+        <v>5661</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>5399</v>
@@ -20157,7 +20169,7 @@
         <v>269</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>5663</v>
+        <v>5662</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>5400</v>
@@ -20174,7 +20186,7 @@
         <v>271</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>5664</v>
+        <v>5663</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>5401</v>
@@ -20191,7 +20203,7 @@
         <v>273</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>5665</v>
+        <v>5664</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>5402</v>
@@ -20225,7 +20237,7 @@
         <v>277</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>5666</v>
+        <v>5665</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>5404</v>
@@ -20242,7 +20254,7 @@
         <v>279</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>5667</v>
+        <v>5666</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>5405</v>
@@ -20259,7 +20271,7 @@
         <v>281</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>5668</v>
+        <v>5667</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>5406</v>
@@ -20276,7 +20288,7 @@
         <v>283</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>5669</v>
+        <v>5668</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>5407</v>
@@ -20293,7 +20305,7 @@
         <v>285</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>5670</v>
+        <v>5669</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>5408</v>
@@ -20315,7 +20327,7 @@
         <v>309</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>5671</v>
+        <v>5670</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>5409</v>
@@ -20332,7 +20344,7 @@
         <v>311</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>5672</v>
+        <v>5671</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>5412</v>
@@ -20349,7 +20361,7 @@
         <v>313</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>5673</v>
+        <v>5672</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>5410</v>
@@ -20366,7 +20378,7 @@
         <v>315</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>5674</v>
+        <v>5673</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>5411</v>
@@ -20400,7 +20412,7 @@
         <v>319</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>5675</v>
+        <v>5674</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>5414</v>
@@ -20417,7 +20429,7 @@
         <v>321</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>5676</v>
+        <v>5675</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>5415</v>
@@ -20434,7 +20446,7 @@
         <v>323</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>5677</v>
+        <v>5676</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>5416</v>
@@ -20451,7 +20463,7 @@
         <v>325</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>5678</v>
+        <v>5677</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>5417</v>
@@ -20468,7 +20480,7 @@
         <v>327</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>5679</v>
+        <v>5678</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>5418</v>
@@ -20502,7 +20514,7 @@
         <v>331</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>5680</v>
+        <v>5679</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>5420</v>
@@ -20519,7 +20531,7 @@
         <v>333</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>5681</v>
+        <v>5680</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>5421</v>
@@ -20536,7 +20548,7 @@
         <v>335</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>5682</v>
+        <v>5681</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>5422</v>
@@ -20553,7 +20565,7 @@
         <v>337</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>5683</v>
+        <v>5682</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>5423</v>
@@ -20570,7 +20582,7 @@
         <v>339</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>5684</v>
+        <v>5683</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>5427</v>
@@ -20587,7 +20599,7 @@
         <v>341</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>5685</v>
+        <v>5684</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>5428</v>
@@ -20604,7 +20616,7 @@
         <v>343</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>5686</v>
+        <v>5685</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>5429</v>
@@ -20621,7 +20633,7 @@
         <v>345</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>5687</v>
+        <v>5686</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>5430</v>
@@ -20638,7 +20650,7 @@
         <v>347</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>5688</v>
+        <v>5687</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>5431</v>
@@ -20655,7 +20667,7 @@
         <v>349</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>5689</v>
+        <v>5688</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>5432</v>
@@ -20672,7 +20684,7 @@
         <v>351</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>5690</v>
+        <v>5689</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>5433</v>
@@ -20689,7 +20701,7 @@
         <v>353</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>5691</v>
+        <v>5690</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>5434</v>
@@ -20706,7 +20718,7 @@
         <v>355</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>5692</v>
+        <v>5691</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>5435</v>
@@ -20723,7 +20735,7 @@
         <v>357</v>
       </c>
       <c r="E140" s="7" t="s">
-        <v>5693</v>
+        <v>5692</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>5436</v>
@@ -20740,7 +20752,7 @@
         <v>359</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>5694</v>
+        <v>5693</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>5437</v>
@@ -20757,7 +20769,7 @@
         <v>361</v>
       </c>
       <c r="E142" s="7" t="s">
-        <v>5695</v>
+        <v>5694</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>5438</v>
@@ -20791,7 +20803,7 @@
         <v>365</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>5696</v>
+        <v>5695</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>5440</v>
@@ -20808,7 +20820,7 @@
         <v>367</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>5697</v>
+        <v>5696</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>5441</v>
@@ -20825,7 +20837,7 @@
         <v>369</v>
       </c>
       <c r="E146" s="7" t="s">
-        <v>5698</v>
+        <v>5697</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>5442</v>
@@ -20842,7 +20854,7 @@
         <v>371</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>5699</v>
+        <v>5698</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>5443</v>
@@ -20859,7 +20871,7 @@
         <v>373</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>5700</v>
+        <v>5699</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>5444</v>
@@ -20876,7 +20888,7 @@
         <v>375</v>
       </c>
       <c r="E149" s="7" t="s">
-        <v>5701</v>
+        <v>5700</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>5445</v>
@@ -20893,7 +20905,7 @@
         <v>377</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>5702</v>
+        <v>5701</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>5446</v>
@@ -20910,7 +20922,7 @@
         <v>379</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>5703</v>
+        <v>5702</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>5447</v>
@@ -20927,7 +20939,7 @@
         <v>381</v>
       </c>
       <c r="E152" s="7" t="s">
-        <v>5704</v>
+        <v>5703</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>5448</v>
@@ -20944,7 +20956,7 @@
         <v>383</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>5705</v>
+        <v>5704</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>5449</v>
@@ -20961,10 +20973,10 @@
         <v>384</v>
       </c>
       <c r="E154" s="7" t="s">
-        <v>5706</v>
+        <v>5964</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>5450</v>
+        <v>5963</v>
       </c>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.6">
@@ -20978,10 +20990,10 @@
         <v>386</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>5707</v>
+        <v>5705</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>5451</v>
+        <v>5450</v>
       </c>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.6">
@@ -20995,10 +21007,10 @@
         <v>388</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>5708</v>
+        <v>5706</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>5452</v>
+        <v>5451</v>
       </c>
     </row>
     <row r="157" spans="2:6" x14ac:dyDescent="0.6">
@@ -21012,10 +21024,10 @@
         <v>390</v>
       </c>
       <c r="E157" s="7" t="s">
-        <v>5709</v>
+        <v>5707</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>5453</v>
+        <v>5452</v>
       </c>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.6">
@@ -21029,10 +21041,10 @@
         <v>392</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>5710</v>
+        <v>5708</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>5454</v>
+        <v>5453</v>
       </c>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.6">
@@ -21046,10 +21058,10 @@
         <v>394</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>5711</v>
+        <v>5709</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>5455</v>
+        <v>5454</v>
       </c>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.6">
@@ -21063,10 +21075,10 @@
         <v>396</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>5712</v>
+        <v>5710</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>5456</v>
+        <v>5455</v>
       </c>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.6">
@@ -21080,10 +21092,10 @@
         <v>398</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>5713</v>
+        <v>5711</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>5457</v>
+        <v>5456</v>
       </c>
     </row>
     <row r="162" spans="2:6" x14ac:dyDescent="0.6">
@@ -21097,10 +21109,10 @@
         <v>400</v>
       </c>
       <c r="E162" s="7" t="s">
-        <v>5714</v>
+        <v>5712</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>5458</v>
+        <v>5457</v>
       </c>
     </row>
     <row r="163" spans="2:6" x14ac:dyDescent="0.6">
@@ -21114,10 +21126,10 @@
         <v>402</v>
       </c>
       <c r="E163" s="7" t="s">
-        <v>5715</v>
+        <v>5713</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>5459</v>
+        <v>5458</v>
       </c>
     </row>
     <row r="164" spans="2:6" x14ac:dyDescent="0.6">
@@ -21131,10 +21143,10 @@
         <v>404</v>
       </c>
       <c r="E164" s="7" t="s">
-        <v>5716</v>
+        <v>5714</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>5460</v>
+        <v>5459</v>
       </c>
     </row>
     <row r="165" spans="2:6" x14ac:dyDescent="0.6">
@@ -21148,10 +21160,10 @@
         <v>406</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>5717</v>
+        <v>5715</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>5461</v>
+        <v>5460</v>
       </c>
     </row>
     <row r="166" spans="2:6" x14ac:dyDescent="0.6">
@@ -21165,10 +21177,10 @@
         <v>408</v>
       </c>
       <c r="E166" s="7" t="s">
-        <v>5718</v>
+        <v>5716</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>5462</v>
+        <v>5461</v>
       </c>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.6">
@@ -21182,10 +21194,10 @@
         <v>410</v>
       </c>
       <c r="E167" s="7" t="s">
-        <v>5719</v>
+        <v>5717</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>5463</v>
+        <v>5462</v>
       </c>
     </row>
     <row r="168" spans="2:6" x14ac:dyDescent="0.6">
@@ -21199,10 +21211,10 @@
         <v>412</v>
       </c>
       <c r="E168" s="7" t="s">
-        <v>5720</v>
+        <v>5718</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>5464</v>
+        <v>5463</v>
       </c>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.6">
@@ -21216,10 +21228,10 @@
         <v>414</v>
       </c>
       <c r="E169" s="7" t="s">
-        <v>5721</v>
+        <v>5719</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>5465</v>
+        <v>5464</v>
       </c>
     </row>
     <row r="170" spans="2:6" x14ac:dyDescent="0.6">
@@ -21233,10 +21245,10 @@
         <v>416</v>
       </c>
       <c r="E170" s="7" t="s">
-        <v>5722</v>
+        <v>5720</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>5466</v>
+        <v>5465</v>
       </c>
     </row>
     <row r="171" spans="2:6" x14ac:dyDescent="0.6">
@@ -21250,10 +21262,10 @@
         <v>418</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>5723</v>
+        <v>5721</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>5467</v>
+        <v>5466</v>
       </c>
     </row>
     <row r="172" spans="2:6" x14ac:dyDescent="0.6">
@@ -21267,10 +21279,10 @@
         <v>420</v>
       </c>
       <c r="E172" s="7" t="s">
-        <v>5724</v>
+        <v>5722</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>5468</v>
+        <v>5467</v>
       </c>
     </row>
     <row r="173" spans="2:6" x14ac:dyDescent="0.6">
@@ -21284,10 +21296,10 @@
         <v>422</v>
       </c>
       <c r="E173" s="7" t="s">
-        <v>5725</v>
+        <v>5723</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>5469</v>
+        <v>5468</v>
       </c>
     </row>
     <row r="174" spans="2:6" x14ac:dyDescent="0.6">
@@ -21301,10 +21313,10 @@
         <v>424</v>
       </c>
       <c r="E174" s="7" t="s">
-        <v>5726</v>
+        <v>5724</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>5470</v>
+        <v>5469</v>
       </c>
     </row>
     <row r="175" spans="2:6" x14ac:dyDescent="0.6">
@@ -21318,10 +21330,10 @@
         <v>426</v>
       </c>
       <c r="E175" s="7" t="s">
-        <v>5727</v>
+        <v>5725</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>5471</v>
+        <v>5470</v>
       </c>
     </row>
     <row r="176" spans="2:6" x14ac:dyDescent="0.6">
@@ -21335,10 +21347,10 @@
         <v>428</v>
       </c>
       <c r="E176" s="7" t="s">
-        <v>5728</v>
+        <v>5726</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>5472</v>
+        <v>5471</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.6">
@@ -21352,10 +21364,10 @@
         <v>430</v>
       </c>
       <c r="E177" s="7" t="s">
-        <v>5729</v>
+        <v>5727</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>5473</v>
+        <v>5472</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.6">
@@ -21369,10 +21381,10 @@
         <v>432</v>
       </c>
       <c r="E178" s="7" t="s">
-        <v>5730</v>
+        <v>5728</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>5474</v>
+        <v>5473</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.6">
@@ -21386,10 +21398,10 @@
         <v>434</v>
       </c>
       <c r="E179" s="7" t="s">
-        <v>5731</v>
+        <v>5729</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>5475</v>
+        <v>5474</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.6">
@@ -21403,10 +21415,10 @@
         <v>436</v>
       </c>
       <c r="E180" s="7" t="s">
-        <v>5732</v>
+        <v>5730</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>5476</v>
+        <v>5475</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.6">
@@ -21420,10 +21432,10 @@
         <v>438</v>
       </c>
       <c r="E181" s="7" t="s">
-        <v>5733</v>
+        <v>5731</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>5477</v>
+        <v>5476</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.6">
@@ -21437,10 +21449,10 @@
         <v>440</v>
       </c>
       <c r="E182" s="7" t="s">
-        <v>5734</v>
+        <v>5732</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>5478</v>
+        <v>5477</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.6">
@@ -21454,10 +21466,10 @@
         <v>442</v>
       </c>
       <c r="E183" s="7" t="s">
-        <v>5479</v>
+        <v>5478</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>5479</v>
+        <v>5478</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.6">
@@ -21471,10 +21483,10 @@
         <v>444</v>
       </c>
       <c r="E184" s="7" t="s">
-        <v>5735</v>
+        <v>5733</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>5480</v>
+        <v>5479</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.6">
@@ -21493,10 +21505,10 @@
         <v>507</v>
       </c>
       <c r="E187" s="7" t="s">
-        <v>5736</v>
+        <v>5734</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>5484</v>
+        <v>5483</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.6">
@@ -21510,10 +21522,10 @@
         <v>281</v>
       </c>
       <c r="E188" s="7" t="s">
-        <v>5737</v>
+        <v>5735</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>5485</v>
+        <v>5484</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.6">
@@ -21527,10 +21539,10 @@
         <v>509</v>
       </c>
       <c r="E189" s="7" t="s">
-        <v>5738</v>
+        <v>5736</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>5486</v>
+        <v>5485</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.6">
@@ -21544,10 +21556,10 @@
         <v>520</v>
       </c>
       <c r="E190" s="7" t="s">
-        <v>5739</v>
+        <v>5737</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>5487</v>
+        <v>5486</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.6">
@@ -21558,13 +21570,13 @@
         <v>521</v>
       </c>
       <c r="D191" s="1" t="s">
+        <v>5492</v>
+      </c>
+      <c r="E191" s="7" t="s">
+        <v>5738</v>
+      </c>
+      <c r="F191" s="1" t="s">
         <v>5493</v>
-      </c>
-      <c r="E191" s="7" t="s">
-        <v>5740</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>5494</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.6">
@@ -21578,10 +21590,10 @@
         <v>512</v>
       </c>
       <c r="E192" s="7" t="s">
-        <v>5741</v>
+        <v>5739</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>5488</v>
+        <v>5487</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.6">
@@ -21595,10 +21607,10 @@
         <v>514</v>
       </c>
       <c r="E193" s="7" t="s">
-        <v>5742</v>
+        <v>5740</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>5489</v>
+        <v>5488</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.6">
@@ -21612,10 +21624,10 @@
         <v>516</v>
       </c>
       <c r="E194" s="7" t="s">
-        <v>5743</v>
+        <v>5741</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>5490</v>
+        <v>5489</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.6">
@@ -21629,10 +21641,10 @@
         <v>518</v>
       </c>
       <c r="E195" s="7" t="s">
-        <v>5744</v>
+        <v>5742</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>5491</v>
+        <v>5490</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.6">
@@ -21646,10 +21658,10 @@
         <v>522</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>5745</v>
+        <v>5743</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>5492</v>
+        <v>5491</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.6">
@@ -21668,10 +21680,10 @@
         <v>533</v>
       </c>
       <c r="E199" s="7" t="s">
-        <v>5746</v>
+        <v>5744</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>5495</v>
+        <v>5494</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.6">
@@ -21685,10 +21697,10 @@
         <v>535</v>
       </c>
       <c r="E200" s="7" t="s">
-        <v>5747</v>
+        <v>5745</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>5496</v>
+        <v>5495</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.6">
@@ -21702,10 +21714,10 @@
         <v>537</v>
       </c>
       <c r="E201" s="7" t="s">
-        <v>5748</v>
+        <v>5746</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>5497</v>
+        <v>5496</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.6">
@@ -21719,10 +21731,10 @@
         <v>539</v>
       </c>
       <c r="E202" s="7" t="s">
-        <v>5749</v>
+        <v>5747</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>5498</v>
+        <v>5497</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.6">
@@ -21736,10 +21748,10 @@
         <v>541</v>
       </c>
       <c r="E203" s="7" t="s">
-        <v>5750</v>
+        <v>5748</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>5499</v>
+        <v>5498</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.6">
@@ -21753,10 +21765,10 @@
         <v>543</v>
       </c>
       <c r="E204" s="7" t="s">
-        <v>5751</v>
+        <v>5749</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>5500</v>
+        <v>5499</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.6">
@@ -21770,10 +21782,10 @@
         <v>545</v>
       </c>
       <c r="E205" s="7" t="s">
-        <v>5752</v>
+        <v>5750</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>5501</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.6">
@@ -21787,10 +21799,10 @@
         <v>547</v>
       </c>
       <c r="E206" s="7" t="s">
-        <v>5753</v>
+        <v>5751</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>5502</v>
+        <v>5501</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.6">
@@ -21804,10 +21816,10 @@
         <v>549</v>
       </c>
       <c r="E207" s="7" t="s">
-        <v>5754</v>
+        <v>5752</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>5503</v>
+        <v>5502</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.6">
@@ -21821,10 +21833,10 @@
         <v>551</v>
       </c>
       <c r="E208" s="7" t="s">
-        <v>5755</v>
+        <v>5753</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>5504</v>
+        <v>5503</v>
       </c>
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.6">
@@ -21838,10 +21850,10 @@
         <v>553</v>
       </c>
       <c r="E209" s="7" t="s">
-        <v>5756</v>
+        <v>5754</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>5505</v>
+        <v>5504</v>
       </c>
     </row>
     <row r="210" spans="2:6" x14ac:dyDescent="0.6">
@@ -21855,10 +21867,10 @@
         <v>555</v>
       </c>
       <c r="E210" s="7" t="s">
-        <v>5757</v>
+        <v>5755</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>5506</v>
+        <v>5505</v>
       </c>
     </row>
     <row r="211" spans="2:6" x14ac:dyDescent="0.6">
@@ -21872,10 +21884,10 @@
         <v>557</v>
       </c>
       <c r="E211" s="7" t="s">
-        <v>5758</v>
+        <v>5756</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>5507</v>
+        <v>5506</v>
       </c>
     </row>
     <row r="212" spans="2:6" x14ac:dyDescent="0.6">
@@ -21889,10 +21901,10 @@
         <v>559</v>
       </c>
       <c r="E212" s="7" t="s">
-        <v>5759</v>
+        <v>5757</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>5508</v>
+        <v>5507</v>
       </c>
     </row>
     <row r="213" spans="2:6" x14ac:dyDescent="0.6">
@@ -21906,10 +21918,10 @@
         <v>561</v>
       </c>
       <c r="E213" s="7" t="s">
-        <v>5760</v>
+        <v>5758</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>5509</v>
+        <v>5508</v>
       </c>
     </row>
     <row r="214" spans="2:6" x14ac:dyDescent="0.6">
@@ -21923,10 +21935,10 @@
         <v>563</v>
       </c>
       <c r="E214" s="7" t="s">
-        <v>5761</v>
+        <v>5759</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>5510</v>
+        <v>5509</v>
       </c>
     </row>
     <row r="215" spans="2:6" x14ac:dyDescent="0.6">
@@ -21940,10 +21952,10 @@
         <v>565</v>
       </c>
       <c r="E215" s="7" t="s">
-        <v>5762</v>
+        <v>5760</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>5511</v>
+        <v>5510</v>
       </c>
     </row>
     <row r="216" spans="2:6" x14ac:dyDescent="0.6">
@@ -21957,10 +21969,10 @@
         <v>567</v>
       </c>
       <c r="E216" s="7" t="s">
-        <v>5763</v>
+        <v>5761</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>5512</v>
+        <v>5511</v>
       </c>
     </row>
     <row r="217" spans="2:6" x14ac:dyDescent="0.6">
@@ -21974,10 +21986,10 @@
         <v>569</v>
       </c>
       <c r="E217" s="7" t="s">
-        <v>5513</v>
+        <v>5512</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>5513</v>
+        <v>5512</v>
       </c>
     </row>
     <row r="218" spans="2:6" x14ac:dyDescent="0.6">
@@ -21991,10 +22003,10 @@
         <v>571</v>
       </c>
       <c r="E218" s="7" t="s">
-        <v>5764</v>
+        <v>5762</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>5514</v>
+        <v>5513</v>
       </c>
     </row>
     <row r="219" spans="2:6" x14ac:dyDescent="0.6">
@@ -22008,10 +22020,10 @@
         <v>573</v>
       </c>
       <c r="E219" s="7" t="s">
-        <v>5765</v>
+        <v>5763</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>5515</v>
+        <v>5514</v>
       </c>
     </row>
     <row r="220" spans="2:6" x14ac:dyDescent="0.6">
@@ -22025,10 +22037,10 @@
         <v>575</v>
       </c>
       <c r="E220" s="7" t="s">
-        <v>5766</v>
+        <v>5764</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>5516</v>
+        <v>5515</v>
       </c>
     </row>
     <row r="221" spans="2:6" x14ac:dyDescent="0.6">
@@ -22042,10 +22054,10 @@
         <v>577</v>
       </c>
       <c r="E221" s="7" t="s">
-        <v>5767</v>
+        <v>5765</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>5517</v>
+        <v>5516</v>
       </c>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.6">
@@ -22059,10 +22071,10 @@
         <v>579</v>
       </c>
       <c r="E222" s="7" t="s">
-        <v>5518</v>
+        <v>5517</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>5518</v>
+        <v>5517</v>
       </c>
     </row>
     <row r="223" spans="2:6" x14ac:dyDescent="0.6">
@@ -22076,10 +22088,10 @@
         <v>581</v>
       </c>
       <c r="E223" s="7" t="s">
-        <v>5768</v>
+        <v>5766</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>5519</v>
+        <v>5518</v>
       </c>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.6">
@@ -22093,10 +22105,10 @@
         <v>583</v>
       </c>
       <c r="E224" s="7" t="s">
-        <v>5769</v>
+        <v>5767</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>5520</v>
+        <v>5519</v>
       </c>
     </row>
     <row r="225" spans="2:6" x14ac:dyDescent="0.6">
@@ -22110,10 +22122,10 @@
         <v>585</v>
       </c>
       <c r="E225" s="7" t="s">
-        <v>5521</v>
+        <v>5520</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>5521</v>
+        <v>5520</v>
       </c>
     </row>
     <row r="226" spans="2:6" x14ac:dyDescent="0.6">
@@ -22127,10 +22139,10 @@
         <v>587</v>
       </c>
       <c r="E226" s="7" t="s">
-        <v>5770</v>
+        <v>5768</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>5522</v>
+        <v>5521</v>
       </c>
     </row>
     <row r="227" spans="2:6" x14ac:dyDescent="0.6">
@@ -22144,10 +22156,10 @@
         <v>589</v>
       </c>
       <c r="E227" s="7" t="s">
-        <v>5771</v>
+        <v>5769</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>5524</v>
+        <v>5523</v>
       </c>
     </row>
     <row r="228" spans="2:6" x14ac:dyDescent="0.6">
@@ -22161,10 +22173,10 @@
         <v>591</v>
       </c>
       <c r="E228" s="7" t="s">
-        <v>5772</v>
+        <v>5770</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>5523</v>
+        <v>5522</v>
       </c>
     </row>
     <row r="229" spans="2:6" x14ac:dyDescent="0.6">
@@ -22178,10 +22190,10 @@
         <v>593</v>
       </c>
       <c r="E229" s="7" t="s">
-        <v>5773</v>
+        <v>5771</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>5525</v>
+        <v>5524</v>
       </c>
     </row>
     <row r="230" spans="2:6" x14ac:dyDescent="0.6">
@@ -22192,13 +22204,13 @@
         <v>595</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>5529</v>
+        <v>5528</v>
       </c>
       <c r="E230" s="7" t="s">
-        <v>5526</v>
+        <v>5525</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>5526</v>
+        <v>5525</v>
       </c>
     </row>
     <row r="231" spans="2:6" x14ac:dyDescent="0.6">
@@ -22209,13 +22221,13 @@
         <v>595</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>5528</v>
+        <v>5527</v>
       </c>
       <c r="E231" s="7" t="s">
-        <v>5527</v>
+        <v>5526</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>5527</v>
+        <v>5526</v>
       </c>
     </row>
     <row r="232" spans="2:6" x14ac:dyDescent="0.6">
@@ -22229,10 +22241,10 @@
         <v>596</v>
       </c>
       <c r="E232" s="7" t="s">
-        <v>5774</v>
+        <v>5772</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>5530</v>
+        <v>5529</v>
       </c>
     </row>
     <row r="233" spans="2:6" x14ac:dyDescent="0.6">
@@ -22246,10 +22258,10 @@
         <v>598</v>
       </c>
       <c r="E233" s="7" t="s">
-        <v>5775</v>
+        <v>5773</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>5531</v>
+        <v>5530</v>
       </c>
     </row>
     <row r="234" spans="2:6" x14ac:dyDescent="0.6">
@@ -22263,10 +22275,10 @@
         <v>600</v>
       </c>
       <c r="E234" s="7" t="s">
-        <v>5776</v>
+        <v>5774</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>5532</v>
+        <v>5531</v>
       </c>
     </row>
     <row r="235" spans="2:6" x14ac:dyDescent="0.6">
@@ -22280,10 +22292,10 @@
         <v>602</v>
       </c>
       <c r="E235" s="7" t="s">
-        <v>5777</v>
+        <v>5775</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>5533</v>
+        <v>5532</v>
       </c>
     </row>
     <row r="236" spans="2:6" x14ac:dyDescent="0.6">
@@ -22297,10 +22309,10 @@
         <v>604</v>
       </c>
       <c r="E236" s="7" t="s">
-        <v>5778</v>
+        <v>5776</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>5534</v>
+        <v>5533</v>
       </c>
     </row>
     <row r="237" spans="2:6" x14ac:dyDescent="0.6">
@@ -22314,10 +22326,10 @@
         <v>606</v>
       </c>
       <c r="E237" s="7" t="s">
-        <v>5779</v>
+        <v>5777</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>5535</v>
+        <v>5534</v>
       </c>
     </row>
     <row r="238" spans="2:6" x14ac:dyDescent="0.6">
@@ -22331,10 +22343,10 @@
         <v>608</v>
       </c>
       <c r="E238" s="7" t="s">
-        <v>5780</v>
+        <v>5778</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>5536</v>
+        <v>5535</v>
       </c>
     </row>
     <row r="239" spans="2:6" x14ac:dyDescent="0.6">
@@ -22348,10 +22360,10 @@
         <v>610</v>
       </c>
       <c r="E239" s="7" t="s">
-        <v>5781</v>
+        <v>5779</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>5537</v>
+        <v>5536</v>
       </c>
     </row>
     <row r="240" spans="2:6" x14ac:dyDescent="0.6">
@@ -22365,10 +22377,10 @@
         <v>612</v>
       </c>
       <c r="E240" s="7" t="s">
-        <v>5782</v>
+        <v>5780</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>5538</v>
+        <v>5537</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.6">
@@ -22382,10 +22394,10 @@
         <v>614</v>
       </c>
       <c r="E241" s="7" t="s">
-        <v>5783</v>
+        <v>5781</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>5539</v>
+        <v>5538</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.6">
@@ -22399,10 +22411,10 @@
         <v>616</v>
       </c>
       <c r="E242" s="7" t="s">
-        <v>5784</v>
+        <v>5782</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>5540</v>
+        <v>5539</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.6">
@@ -22416,10 +22428,10 @@
         <v>618</v>
       </c>
       <c r="E243" s="7" t="s">
-        <v>5785</v>
+        <v>5783</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>5547</v>
+        <v>5546</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.6">
@@ -22433,10 +22445,10 @@
         <v>620</v>
       </c>
       <c r="E244" s="7" t="s">
-        <v>5786</v>
+        <v>5784</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>5545</v>
+        <v>5544</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.6">
@@ -22450,10 +22462,10 @@
         <v>622</v>
       </c>
       <c r="E245" s="7" t="s">
-        <v>5787</v>
+        <v>5785</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>5541</v>
+        <v>5540</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.6">
@@ -22467,10 +22479,10 @@
         <v>624</v>
       </c>
       <c r="E246" s="7" t="s">
-        <v>5788</v>
+        <v>5786</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>5542</v>
+        <v>5541</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.6">
@@ -22484,10 +22496,10 @@
         <v>626</v>
       </c>
       <c r="E247" s="7" t="s">
-        <v>5789</v>
+        <v>5787</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>5543</v>
+        <v>5542</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.6">
@@ -22501,10 +22513,10 @@
         <v>628</v>
       </c>
       <c r="E248" s="7" t="s">
-        <v>5790</v>
+        <v>5788</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>5544</v>
+        <v>5543</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.6">
@@ -22518,10 +22530,10 @@
         <v>630</v>
       </c>
       <c r="E249" s="7" t="s">
-        <v>5791</v>
+        <v>5789</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>5546</v>
+        <v>5545</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.6">
@@ -22535,10 +22547,10 @@
         <v>632</v>
       </c>
       <c r="E250" s="7" t="s">
-        <v>5792</v>
+        <v>5790</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>5548</v>
+        <v>5547</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.6">
@@ -22552,10 +22564,10 @@
         <v>634</v>
       </c>
       <c r="E251" s="7" t="s">
-        <v>5793</v>
+        <v>5791</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>5549</v>
+        <v>5548</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.6">
@@ -22569,10 +22581,10 @@
         <v>636</v>
       </c>
       <c r="E252" s="7" t="s">
-        <v>5794</v>
+        <v>5792</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>5550</v>
+        <v>5549</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.6">
@@ -22591,10 +22603,10 @@
         <v>675</v>
       </c>
       <c r="E255" s="7" t="s">
-        <v>5795</v>
+        <v>5793</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>5551</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.6">
@@ -22608,10 +22620,10 @@
         <v>677</v>
       </c>
       <c r="E256" s="7" t="s">
-        <v>5796</v>
+        <v>5794</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>5552</v>
+        <v>5551</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.6">
@@ -22625,10 +22637,10 @@
         <v>679</v>
       </c>
       <c r="E257" s="7" t="s">
-        <v>5797</v>
+        <v>5795</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>5553</v>
+        <v>5552</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.6">
@@ -22642,10 +22654,10 @@
         <v>681</v>
       </c>
       <c r="E258" s="7" t="s">
-        <v>5798</v>
+        <v>5796</v>
       </c>
       <c r="F258" s="1" t="s">
-        <v>5555</v>
+        <v>5554</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.6">
@@ -22659,10 +22671,10 @@
         <v>683</v>
       </c>
       <c r="E259" s="7" t="s">
-        <v>5799</v>
+        <v>5797</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>5554</v>
+        <v>5553</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.6">
@@ -22676,10 +22688,10 @@
         <v>685</v>
       </c>
       <c r="E260" s="7" t="s">
-        <v>5800</v>
+        <v>5798</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>5556</v>
+        <v>5555</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.6">
@@ -22693,10 +22705,10 @@
         <v>687</v>
       </c>
       <c r="E261" s="7" t="s">
-        <v>5801</v>
+        <v>5799</v>
       </c>
       <c r="F261" s="1" t="s">
-        <v>5557</v>
+        <v>5556</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.6">
@@ -22710,10 +22722,10 @@
         <v>689</v>
       </c>
       <c r="E262" s="7" t="s">
-        <v>5802</v>
+        <v>5800</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>5558</v>
+        <v>5557</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.6">
@@ -22727,10 +22739,10 @@
         <v>691</v>
       </c>
       <c r="E263" s="7" t="s">
-        <v>5803</v>
+        <v>5801</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>5559</v>
+        <v>5558</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.6">
@@ -22744,10 +22756,10 @@
         <v>693</v>
       </c>
       <c r="E264" s="7" t="s">
-        <v>5804</v>
+        <v>5802</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>5560</v>
+        <v>5559</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.6">
@@ -22761,10 +22773,10 @@
         <v>695</v>
       </c>
       <c r="E265" s="7" t="s">
-        <v>5805</v>
+        <v>5803</v>
       </c>
       <c r="F265" s="1" t="s">
-        <v>5561</v>
+        <v>5560</v>
       </c>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.6">
@@ -22778,10 +22790,10 @@
         <v>697</v>
       </c>
       <c r="E266" s="7" t="s">
-        <v>5806</v>
+        <v>5804</v>
       </c>
       <c r="F266" s="1" t="s">
-        <v>5562</v>
+        <v>5561</v>
       </c>
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.6">
@@ -22795,10 +22807,10 @@
         <v>699</v>
       </c>
       <c r="E267" s="7" t="s">
-        <v>5563</v>
+        <v>5562</v>
       </c>
       <c r="F267" s="1" t="s">
-        <v>5563</v>
+        <v>5562</v>
       </c>
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.6">
@@ -22812,10 +22824,10 @@
         <v>701</v>
       </c>
       <c r="E268" s="7" t="s">
-        <v>5807</v>
+        <v>5805</v>
       </c>
       <c r="F268" s="1" t="s">
-        <v>5564</v>
+        <v>5563</v>
       </c>
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.6">
@@ -22829,10 +22841,10 @@
         <v>703</v>
       </c>
       <c r="E269" s="7" t="s">
-        <v>5565</v>
+        <v>5564</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>5565</v>
+        <v>5564</v>
       </c>
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.6">
@@ -22846,10 +22858,10 @@
         <v>705</v>
       </c>
       <c r="E270" s="7" t="s">
-        <v>5563</v>
+        <v>5562</v>
       </c>
       <c r="F270" s="1" t="s">
-        <v>5563</v>
+        <v>5562</v>
       </c>
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.6">
@@ -22863,10 +22875,10 @@
         <v>707</v>
       </c>
       <c r="E271" s="7" t="s">
-        <v>5808</v>
+        <v>5806</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>5566</v>
+        <v>5565</v>
       </c>
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.6">
@@ -22880,10 +22892,10 @@
         <v>709</v>
       </c>
       <c r="E272" s="7" t="s">
-        <v>5809</v>
+        <v>5807</v>
       </c>
       <c r="F272" s="1" t="s">
-        <v>5567</v>
+        <v>5566</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.6">
@@ -22897,10 +22909,10 @@
         <v>711</v>
       </c>
       <c r="E273" s="7" t="s">
-        <v>5810</v>
+        <v>5808</v>
       </c>
       <c r="F273" s="1" t="s">
-        <v>5568</v>
+        <v>5567</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.6">
@@ -22914,10 +22926,10 @@
         <v>713</v>
       </c>
       <c r="E274" s="7" t="s">
-        <v>5811</v>
+        <v>5809</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>5569</v>
+        <v>5568</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.6">
@@ -22931,10 +22943,10 @@
         <v>715</v>
       </c>
       <c r="E275" s="7" t="s">
-        <v>5812</v>
+        <v>5810</v>
       </c>
       <c r="F275" s="1" t="s">
-        <v>5570</v>
+        <v>5569</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.6">
@@ -22948,44 +22960,44 @@
         <v>717</v>
       </c>
       <c r="E276" s="7" t="s">
-        <v>5813</v>
+        <v>5811</v>
       </c>
       <c r="F276" s="1" t="s">
-        <v>5571</v>
+        <v>5570</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.6">
       <c r="B277" s="1" t="s">
+        <v>5573</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>5573</v>
+      </c>
+      <c r="D277" s="1" t="s">
         <v>5574</v>
       </c>
-      <c r="C277" s="1" t="s">
-        <v>5574</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>5575</v>
-      </c>
       <c r="E277" s="7" t="s">
-        <v>5814</v>
+        <v>5812</v>
       </c>
       <c r="F277" s="1" t="s">
-        <v>5572</v>
+        <v>5571</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.6">
       <c r="B278" s="1" t="s">
+        <v>5575</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>5575</v>
+      </c>
+      <c r="D278" s="1" t="s">
         <v>5576</v>
       </c>
-      <c r="C278" s="1" t="s">
-        <v>5576</v>
-      </c>
-      <c r="D278" s="1" t="s">
+      <c r="E278" s="7" t="s">
+        <v>5813</v>
+      </c>
+      <c r="F278" s="1" t="s">
         <v>5577</v>
-      </c>
-      <c r="E278" s="7" t="s">
-        <v>5815</v>
-      </c>
-      <c r="F278" s="1" t="s">
-        <v>5578</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.6">
@@ -22999,10 +23011,10 @@
         <v>719</v>
       </c>
       <c r="E279" s="7" t="s">
-        <v>5816</v>
+        <v>5814</v>
       </c>
       <c r="F279" s="1" t="s">
-        <v>5573</v>
+        <v>5572</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.6">
@@ -23021,7 +23033,7 @@
         <v>728</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>5821</v>
+        <v>5819</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.6">
@@ -23035,7 +23047,7 @@
         <v>730</v>
       </c>
       <c r="F283" s="1" t="s">
-        <v>5822</v>
+        <v>5820</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.6">
@@ -23049,7 +23061,7 @@
         <v>732</v>
       </c>
       <c r="F284" s="1" t="s">
-        <v>5823</v>
+        <v>5821</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.6">
@@ -23063,7 +23075,7 @@
         <v>734</v>
       </c>
       <c r="F285" s="1" t="s">
-        <v>5824</v>
+        <v>5822</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.6">
@@ -23077,7 +23089,7 @@
         <v>736</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>5825</v>
+        <v>5823</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.6">
@@ -23091,7 +23103,7 @@
         <v>738</v>
       </c>
       <c r="F287" s="1" t="s">
-        <v>5826</v>
+        <v>5824</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.6">
@@ -23105,7 +23117,7 @@
         <v>740</v>
       </c>
       <c r="F288" s="1" t="s">
-        <v>5827</v>
+        <v>5825</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.6">
@@ -23119,7 +23131,7 @@
         <v>742</v>
       </c>
       <c r="F289" s="1" t="s">
-        <v>5828</v>
+        <v>5826</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.6">
@@ -23130,7 +23142,7 @@
         <v>744</v>
       </c>
       <c r="F290" s="1" t="s">
-        <v>5829</v>
+        <v>5827</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.6">
@@ -23144,7 +23156,7 @@
         <v>746</v>
       </c>
       <c r="F291" s="1" t="s">
-        <v>5830</v>
+        <v>5828</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.6">
@@ -23158,7 +23170,7 @@
         <v>748</v>
       </c>
       <c r="F292" s="1" t="s">
-        <v>5831</v>
+        <v>5829</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.6">
@@ -23172,7 +23184,7 @@
         <v>750</v>
       </c>
       <c r="F293" s="1" t="s">
-        <v>5832</v>
+        <v>5830</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.6">
@@ -23186,7 +23198,7 @@
         <v>752</v>
       </c>
       <c r="F294" s="1" t="s">
-        <v>5833</v>
+        <v>5831</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.6">
@@ -23205,7 +23217,7 @@
         <v>766</v>
       </c>
       <c r="F297" s="1" t="s">
-        <v>5834</v>
+        <v>5832</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.6">
@@ -23219,7 +23231,7 @@
         <v>768</v>
       </c>
       <c r="F298" s="1" t="s">
-        <v>5838</v>
+        <v>5836</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.6">
@@ -23233,7 +23245,7 @@
         <v>770</v>
       </c>
       <c r="F299" s="1" t="s">
-        <v>5835</v>
+        <v>5833</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.6">
@@ -23247,7 +23259,7 @@
         <v>772</v>
       </c>
       <c r="F300" s="1" t="s">
-        <v>5839</v>
+        <v>5837</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.6">
@@ -23261,7 +23273,7 @@
         <v>774</v>
       </c>
       <c r="F301" s="1" t="s">
-        <v>5836</v>
+        <v>5834</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.6">
@@ -23275,7 +23287,7 @@
         <v>776</v>
       </c>
       <c r="F302" s="1" t="s">
-        <v>5837</v>
+        <v>5835</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.6">
@@ -23289,12 +23301,12 @@
         <v>778</v>
       </c>
       <c r="F303" s="1" t="s">
-        <v>5840</v>
+        <v>5838</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.6">
       <c r="F304" s="1" t="s">
-        <v>5841</v>
+        <v>5839</v>
       </c>
     </row>
     <row r="305" spans="2:6" x14ac:dyDescent="0.6">
@@ -23308,7 +23320,7 @@
         <v>780</v>
       </c>
       <c r="F305" s="1" t="s">
-        <v>5842</v>
+        <v>5840</v>
       </c>
     </row>
     <row r="306" spans="2:6" x14ac:dyDescent="0.6">
@@ -23322,7 +23334,7 @@
         <v>782</v>
       </c>
       <c r="F306" s="1" t="s">
-        <v>5843</v>
+        <v>5841</v>
       </c>
     </row>
     <row r="307" spans="2:6" x14ac:dyDescent="0.6">
@@ -23336,7 +23348,7 @@
         <v>784</v>
       </c>
       <c r="F307" s="1" t="s">
-        <v>5844</v>
+        <v>5842</v>
       </c>
     </row>
     <row r="308" spans="2:6" x14ac:dyDescent="0.6">
@@ -23350,7 +23362,7 @@
         <v>786</v>
       </c>
       <c r="F308" s="1" t="s">
-        <v>5845</v>
+        <v>5843</v>
       </c>
     </row>
     <row r="309" spans="2:6" x14ac:dyDescent="0.6">
@@ -23364,7 +23376,7 @@
         <v>788</v>
       </c>
       <c r="F309" s="1" t="s">
-        <v>5846</v>
+        <v>5844</v>
       </c>
     </row>
     <row r="310" spans="2:6" x14ac:dyDescent="0.6">
@@ -23378,7 +23390,7 @@
         <v>790</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>5847</v>
+        <v>5845</v>
       </c>
     </row>
     <row r="311" spans="2:6" x14ac:dyDescent="0.6">
@@ -23392,7 +23404,7 @@
         <v>792</v>
       </c>
       <c r="F311" s="1" t="s">
-        <v>5848</v>
+        <v>5846</v>
       </c>
     </row>
     <row r="312" spans="2:6" x14ac:dyDescent="0.6">
@@ -23406,7 +23418,7 @@
         <v>794</v>
       </c>
       <c r="F312" s="1" t="s">
-        <v>5849</v>
+        <v>5847</v>
       </c>
     </row>
     <row r="313" spans="2:6" x14ac:dyDescent="0.6">
@@ -23420,7 +23432,7 @@
         <v>796</v>
       </c>
       <c r="F313" s="1" t="s">
-        <v>5850</v>
+        <v>5848</v>
       </c>
     </row>
     <row r="314" spans="2:6" x14ac:dyDescent="0.6">
@@ -23431,7 +23443,7 @@
         <v>798</v>
       </c>
       <c r="F314" s="1" t="s">
-        <v>5851</v>
+        <v>5849</v>
       </c>
     </row>
     <row r="315" spans="2:6" x14ac:dyDescent="0.6">
@@ -23442,24 +23454,24 @@
         <v>801</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>5856</v>
+        <v>5854</v>
       </c>
       <c r="F315" s="1" t="s">
-        <v>5852</v>
+        <v>5850</v>
       </c>
     </row>
     <row r="316" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B316" s="1" t="s">
-        <v>5854</v>
+        <v>5852</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>5855</v>
+        <v>5853</v>
       </c>
       <c r="D316" s="1" t="s">
         <v>800</v>
       </c>
       <c r="F316" s="1" t="s">
-        <v>5857</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="317" spans="2:6" x14ac:dyDescent="0.6">
@@ -23473,7 +23485,7 @@
         <v>802</v>
       </c>
       <c r="F317" s="1" t="s">
-        <v>5853</v>
+        <v>5851</v>
       </c>
     </row>
     <row r="318" spans="2:6" x14ac:dyDescent="0.6">
@@ -23487,7 +23499,7 @@
         <v>804</v>
       </c>
       <c r="F318" s="1" t="s">
-        <v>5858</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="319" spans="2:6" x14ac:dyDescent="0.6">
@@ -23501,7 +23513,7 @@
         <v>806</v>
       </c>
       <c r="F319" s="1" t="s">
-        <v>5859</v>
+        <v>5857</v>
       </c>
     </row>
     <row r="320" spans="2:6" x14ac:dyDescent="0.6">
@@ -23515,7 +23527,7 @@
         <v>808</v>
       </c>
       <c r="F320" s="1" t="s">
-        <v>5860</v>
+        <v>5858</v>
       </c>
     </row>
     <row r="321" spans="2:6" x14ac:dyDescent="0.6">
@@ -23529,7 +23541,7 @@
         <v>5319</v>
       </c>
       <c r="F321" s="1" t="s">
-        <v>5861</v>
+        <v>5859</v>
       </c>
     </row>
     <row r="322" spans="2:6" x14ac:dyDescent="0.6">
@@ -23543,7 +23555,7 @@
         <v>810</v>
       </c>
       <c r="F322" s="1" t="s">
-        <v>5862</v>
+        <v>5860</v>
       </c>
     </row>
     <row r="323" spans="2:6" x14ac:dyDescent="0.6">
@@ -23557,7 +23569,7 @@
         <v>812</v>
       </c>
       <c r="F323" s="1" t="s">
-        <v>5863</v>
+        <v>5861</v>
       </c>
     </row>
     <row r="324" spans="2:6" x14ac:dyDescent="0.6">
@@ -23571,7 +23583,7 @@
         <v>814</v>
       </c>
       <c r="F324" s="1" t="s">
-        <v>5864</v>
+        <v>5862</v>
       </c>
     </row>
     <row r="325" spans="2:6" x14ac:dyDescent="0.6">
@@ -23585,7 +23597,7 @@
         <v>816</v>
       </c>
       <c r="F325" s="1" t="s">
-        <v>5865</v>
+        <v>5863</v>
       </c>
     </row>
     <row r="326" spans="2:6" x14ac:dyDescent="0.6">
@@ -23599,7 +23611,7 @@
         <v>818</v>
       </c>
       <c r="F326" s="1" t="s">
-        <v>5866</v>
+        <v>5864</v>
       </c>
     </row>
     <row r="327" spans="2:6" x14ac:dyDescent="0.6">
@@ -23613,7 +23625,7 @@
         <v>820</v>
       </c>
       <c r="F327" s="1" t="s">
-        <v>5867</v>
+        <v>5865</v>
       </c>
     </row>
     <row r="328" spans="2:6" x14ac:dyDescent="0.6">
@@ -23624,7 +23636,7 @@
         <v>822</v>
       </c>
       <c r="F328" s="1" t="s">
-        <v>5868</v>
+        <v>5866</v>
       </c>
     </row>
     <row r="329" spans="2:6" x14ac:dyDescent="0.6">
@@ -23635,7 +23647,7 @@
         <v>824</v>
       </c>
       <c r="F329" s="1" t="s">
-        <v>5869</v>
+        <v>5867</v>
       </c>
     </row>
     <row r="330" spans="2:6" x14ac:dyDescent="0.6">
@@ -23646,7 +23658,7 @@
         <v>826</v>
       </c>
       <c r="F330" s="1" t="s">
-        <v>5870</v>
+        <v>5868</v>
       </c>
     </row>
     <row r="331" spans="2:6" x14ac:dyDescent="0.6">
@@ -23657,7 +23669,7 @@
         <v>828</v>
       </c>
       <c r="F331" s="1" t="s">
-        <v>5871</v>
+        <v>5869</v>
       </c>
     </row>
     <row r="332" spans="2:6" x14ac:dyDescent="0.6">
@@ -23671,7 +23683,7 @@
         <v>830</v>
       </c>
       <c r="F332" s="1" t="s">
-        <v>5872</v>
+        <v>5870</v>
       </c>
     </row>
     <row r="333" spans="2:6" x14ac:dyDescent="0.6">
@@ -23685,7 +23697,7 @@
         <v>832</v>
       </c>
       <c r="F333" s="1" t="s">
-        <v>5873</v>
+        <v>5871</v>
       </c>
     </row>
     <row r="334" spans="2:6" x14ac:dyDescent="0.6">
@@ -23696,7 +23708,7 @@
         <v>834</v>
       </c>
       <c r="F334" s="1" t="s">
-        <v>5874</v>
+        <v>5872</v>
       </c>
     </row>
     <row r="335" spans="2:6" x14ac:dyDescent="0.6">
@@ -23707,7 +23719,7 @@
         <v>836</v>
       </c>
       <c r="F335" s="1" t="s">
-        <v>5875</v>
+        <v>5873</v>
       </c>
     </row>
     <row r="336" spans="2:6" x14ac:dyDescent="0.6">
@@ -23718,7 +23730,7 @@
         <v>838</v>
       </c>
       <c r="F336" s="1" t="s">
-        <v>5876</v>
+        <v>5874</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.6">
@@ -23732,7 +23744,7 @@
         <v>840</v>
       </c>
       <c r="F337" s="1" t="s">
-        <v>5877</v>
+        <v>5875</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.6">
@@ -23746,7 +23758,7 @@
         <v>842</v>
       </c>
       <c r="F338" s="1" t="s">
-        <v>5878</v>
+        <v>5876</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.6">
@@ -23760,7 +23772,7 @@
         <v>844</v>
       </c>
       <c r="F339" s="1" t="s">
-        <v>5879</v>
+        <v>5877</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.6">
@@ -23774,7 +23786,7 @@
         <v>846</v>
       </c>
       <c r="F340" s="1" t="s">
-        <v>5880</v>
+        <v>5878</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.6">
@@ -23788,7 +23800,7 @@
         <v>848</v>
       </c>
       <c r="F341" s="1" t="s">
-        <v>5881</v>
+        <v>5879</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.6">
@@ -23802,7 +23814,7 @@
         <v>850</v>
       </c>
       <c r="F342" s="1" t="s">
-        <v>5882</v>
+        <v>5880</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.6">
@@ -23816,7 +23828,7 @@
         <v>852</v>
       </c>
       <c r="F343" s="1" t="s">
-        <v>5883</v>
+        <v>5881</v>
       </c>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.6">
@@ -23830,7 +23842,7 @@
         <v>854</v>
       </c>
       <c r="F344" s="1" t="s">
-        <v>5884</v>
+        <v>5882</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.6">
@@ -23849,7 +23861,7 @@
         <v>893</v>
       </c>
       <c r="F347" s="1" t="s">
-        <v>5885</v>
+        <v>5883</v>
       </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.6">
@@ -23863,7 +23875,7 @@
         <v>895</v>
       </c>
       <c r="F348" s="1" t="s">
-        <v>5886</v>
+        <v>5884</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.6">
@@ -23877,7 +23889,7 @@
         <v>897</v>
       </c>
       <c r="F349" s="1" t="s">
-        <v>5887</v>
+        <v>5885</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.6">
@@ -23891,7 +23903,7 @@
         <v>899</v>
       </c>
       <c r="F350" s="1" t="s">
-        <v>5888</v>
+        <v>5886</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.6">
@@ -23905,7 +23917,7 @@
         <v>901</v>
       </c>
       <c r="F351" s="1" t="s">
-        <v>5889</v>
+        <v>5887</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.6">
@@ -23913,10 +23925,10 @@
         <v>903</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>5891</v>
+        <v>5889</v>
       </c>
       <c r="F352" s="1" t="s">
-        <v>5890</v>
+        <v>5888</v>
       </c>
     </row>
     <row r="353" spans="2:6" x14ac:dyDescent="0.6">
@@ -23924,10 +23936,10 @@
         <v>904</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>5892</v>
+        <v>5890</v>
       </c>
       <c r="F353" s="1" t="s">
-        <v>5893</v>
+        <v>5891</v>
       </c>
     </row>
     <row r="354" spans="2:6" x14ac:dyDescent="0.6">
@@ -23941,7 +23953,7 @@
         <v>905</v>
       </c>
       <c r="F354" s="1" t="s">
-        <v>5902</v>
+        <v>5900</v>
       </c>
     </row>
     <row r="355" spans="2:6" x14ac:dyDescent="0.6">
@@ -23955,7 +23967,7 @@
         <v>907</v>
       </c>
       <c r="F355" s="1" t="s">
-        <v>5894</v>
+        <v>5892</v>
       </c>
     </row>
     <row r="356" spans="2:6" x14ac:dyDescent="0.6">
@@ -23966,7 +23978,7 @@
         <v>909</v>
       </c>
       <c r="F356" s="1" t="s">
-        <v>5896</v>
+        <v>5894</v>
       </c>
     </row>
     <row r="357" spans="2:6" x14ac:dyDescent="0.6">
@@ -23977,7 +23989,7 @@
         <v>911</v>
       </c>
       <c r="F357" s="1" t="s">
-        <v>5895</v>
+        <v>5893</v>
       </c>
     </row>
     <row r="358" spans="2:6" x14ac:dyDescent="0.6">
@@ -23991,7 +24003,7 @@
         <v>913</v>
       </c>
       <c r="F358" s="1" t="s">
-        <v>5897</v>
+        <v>5895</v>
       </c>
     </row>
     <row r="359" spans="2:6" x14ac:dyDescent="0.6">
@@ -24005,7 +24017,7 @@
         <v>915</v>
       </c>
       <c r="F359" s="1" t="s">
-        <v>5898</v>
+        <v>5896</v>
       </c>
     </row>
     <row r="360" spans="2:6" x14ac:dyDescent="0.6">
@@ -24019,7 +24031,7 @@
         <v>917</v>
       </c>
       <c r="F360" s="1" t="s">
-        <v>5899</v>
+        <v>5897</v>
       </c>
     </row>
     <row r="361" spans="2:6" x14ac:dyDescent="0.6">
@@ -24033,7 +24045,7 @@
         <v>919</v>
       </c>
       <c r="F361" s="1" t="s">
-        <v>5900</v>
+        <v>5898</v>
       </c>
     </row>
     <row r="362" spans="2:6" x14ac:dyDescent="0.6">
@@ -24044,7 +24056,7 @@
         <v>921</v>
       </c>
       <c r="F362" s="1" t="s">
-        <v>5901</v>
+        <v>5899</v>
       </c>
     </row>
     <row r="363" spans="2:6" x14ac:dyDescent="0.6">
@@ -24055,7 +24067,7 @@
         <v>923</v>
       </c>
       <c r="F363" s="1" t="s">
-        <v>5903</v>
+        <v>5901</v>
       </c>
     </row>
     <row r="364" spans="2:6" x14ac:dyDescent="0.6">
@@ -24069,7 +24081,7 @@
         <v>925</v>
       </c>
       <c r="F364" s="1" t="s">
-        <v>5904</v>
+        <v>5902</v>
       </c>
     </row>
     <row r="365" spans="2:6" x14ac:dyDescent="0.6">
@@ -24083,7 +24095,7 @@
         <v>927</v>
       </c>
       <c r="F365" s="1" t="s">
-        <v>5905</v>
+        <v>5903</v>
       </c>
     </row>
     <row r="366" spans="2:6" x14ac:dyDescent="0.6">
@@ -24097,7 +24109,7 @@
         <v>929</v>
       </c>
       <c r="F366" s="1" t="s">
-        <v>5906</v>
+        <v>5904</v>
       </c>
     </row>
     <row r="367" spans="2:6" x14ac:dyDescent="0.6">
@@ -24111,7 +24123,7 @@
         <v>931</v>
       </c>
       <c r="F367" s="1" t="s">
-        <v>5907</v>
+        <v>5905</v>
       </c>
     </row>
     <row r="368" spans="2:6" x14ac:dyDescent="0.6">
@@ -24125,7 +24137,7 @@
         <v>933</v>
       </c>
       <c r="F368" s="1" t="s">
-        <v>5908</v>
+        <v>5906</v>
       </c>
     </row>
     <row r="369" spans="2:6" x14ac:dyDescent="0.6">
@@ -24139,7 +24151,7 @@
         <v>935</v>
       </c>
       <c r="F369" s="1" t="s">
-        <v>5909</v>
+        <v>5907</v>
       </c>
     </row>
     <row r="370" spans="2:6" x14ac:dyDescent="0.6">
@@ -24153,7 +24165,7 @@
         <v>937</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>5910</v>
+        <v>5908</v>
       </c>
     </row>
     <row r="371" spans="2:6" x14ac:dyDescent="0.6">
@@ -24164,7 +24176,7 @@
         <v>939</v>
       </c>
       <c r="F371" s="1" t="s">
-        <v>5911</v>
+        <v>5909</v>
       </c>
     </row>
     <row r="372" spans="2:6" x14ac:dyDescent="0.6">
@@ -24178,7 +24190,7 @@
         <v>941</v>
       </c>
       <c r="F372" s="1" t="s">
-        <v>5912</v>
+        <v>5910</v>
       </c>
     </row>
     <row r="373" spans="2:6" x14ac:dyDescent="0.6">
@@ -24192,7 +24204,7 @@
         <v>943</v>
       </c>
       <c r="F373" s="1" t="s">
-        <v>5913</v>
+        <v>5911</v>
       </c>
     </row>
     <row r="374" spans="2:6" x14ac:dyDescent="0.6">
@@ -24203,7 +24215,7 @@
         <v>945</v>
       </c>
       <c r="F374" s="1" t="s">
-        <v>5914</v>
+        <v>5912</v>
       </c>
     </row>
     <row r="375" spans="2:6" x14ac:dyDescent="0.6">
@@ -24214,7 +24226,7 @@
         <v>947</v>
       </c>
       <c r="F375" s="1" t="s">
-        <v>5915</v>
+        <v>5913</v>
       </c>
     </row>
     <row r="376" spans="2:6" x14ac:dyDescent="0.6">
@@ -24225,7 +24237,7 @@
         <v>949</v>
       </c>
       <c r="F376" s="1" t="s">
-        <v>5916</v>
+        <v>5914</v>
       </c>
     </row>
     <row r="377" spans="2:6" x14ac:dyDescent="0.6">
@@ -24239,7 +24251,7 @@
         <v>951</v>
       </c>
       <c r="F377" s="1" t="s">
-        <v>5917</v>
+        <v>5915</v>
       </c>
     </row>
     <row r="378" spans="2:6" x14ac:dyDescent="0.6">
@@ -24253,7 +24265,7 @@
         <v>953</v>
       </c>
       <c r="F378" s="1" t="s">
-        <v>5918</v>
+        <v>5916</v>
       </c>
     </row>
     <row r="379" spans="2:6" x14ac:dyDescent="0.6">
@@ -24267,7 +24279,7 @@
         <v>955</v>
       </c>
       <c r="F379" s="1" t="s">
-        <v>5907</v>
+        <v>5905</v>
       </c>
     </row>
     <row r="380" spans="2:6" x14ac:dyDescent="0.6">
@@ -24281,7 +24293,7 @@
         <v>957</v>
       </c>
       <c r="F380" s="1" t="s">
-        <v>5919</v>
+        <v>5917</v>
       </c>
     </row>
     <row r="381" spans="2:6" x14ac:dyDescent="0.6">
@@ -24295,21 +24307,21 @@
         <v>959</v>
       </c>
       <c r="F381" s="1" t="s">
-        <v>5920</v>
+        <v>5918</v>
       </c>
     </row>
     <row r="382" spans="2:6" x14ac:dyDescent="0.6">
       <c r="B382" s="1" t="s">
+        <v>5920</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>5921</v>
+      </c>
+      <c r="D382" s="1" t="s">
         <v>5922</v>
       </c>
-      <c r="C382" s="1" t="s">
+      <c r="F382" s="1" t="s">
         <v>5923</v>
-      </c>
-      <c r="D382" s="1" t="s">
-        <v>5924</v>
-      </c>
-      <c r="F382" s="1" t="s">
-        <v>5925</v>
       </c>
     </row>
     <row r="383" spans="2:6" x14ac:dyDescent="0.6">
@@ -24323,7 +24335,7 @@
         <v>961</v>
       </c>
       <c r="F383" s="1" t="s">
-        <v>5928</v>
+        <v>5926</v>
       </c>
     </row>
     <row r="384" spans="2:6" x14ac:dyDescent="0.6">
@@ -24337,7 +24349,7 @@
         <v>963</v>
       </c>
       <c r="F384" s="1" t="s">
-        <v>5927</v>
+        <v>5925</v>
       </c>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.6">
@@ -24351,7 +24363,7 @@
         <v>965</v>
       </c>
       <c r="F385" s="1" t="s">
-        <v>5921</v>
+        <v>5919</v>
       </c>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.6">
@@ -24362,7 +24374,7 @@
         <v>967</v>
       </c>
       <c r="F386" s="1" t="s">
-        <v>5926</v>
+        <v>5924</v>
       </c>
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.6">
@@ -24381,7 +24393,7 @@
         <v>997</v>
       </c>
       <c r="F389" s="1" t="s">
-        <v>5929</v>
+        <v>5927</v>
       </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.6">
@@ -24395,7 +24407,7 @@
         <v>999</v>
       </c>
       <c r="F390" s="1" t="s">
-        <v>5930</v>
+        <v>5928</v>
       </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.6">
@@ -24409,7 +24421,7 @@
         <v>1001</v>
       </c>
       <c r="F391" s="1" t="s">
-        <v>5931</v>
+        <v>5929</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.6">
@@ -24423,7 +24435,7 @@
         <v>1003</v>
       </c>
       <c r="F392" s="1" t="s">
-        <v>5932</v>
+        <v>5930</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.6">
@@ -24437,7 +24449,7 @@
         <v>1005</v>
       </c>
       <c r="F393" s="1" t="s">
-        <v>5933</v>
+        <v>5931</v>
       </c>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.6">
@@ -24451,7 +24463,7 @@
         <v>1007</v>
       </c>
       <c r="F394" s="1" t="s">
-        <v>5934</v>
+        <v>5932</v>
       </c>
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.6">
@@ -24465,7 +24477,7 @@
         <v>1009</v>
       </c>
       <c r="F395" s="1" t="s">
-        <v>5935</v>
+        <v>5933</v>
       </c>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.6">
@@ -24479,7 +24491,7 @@
         <v>1011</v>
       </c>
       <c r="F396" s="1" t="s">
-        <v>5936</v>
+        <v>5934</v>
       </c>
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.6">
@@ -24493,7 +24505,7 @@
         <v>1013</v>
       </c>
       <c r="F397" s="1" t="s">
-        <v>5937</v>
+        <v>5935</v>
       </c>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.6">
@@ -24507,7 +24519,7 @@
         <v>1015</v>
       </c>
       <c r="F398" s="1" t="s">
-        <v>5938</v>
+        <v>5936</v>
       </c>
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.6">
@@ -24521,7 +24533,7 @@
         <v>1017</v>
       </c>
       <c r="F399" s="1" t="s">
-        <v>5939</v>
+        <v>5937</v>
       </c>
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.6">
@@ -24532,7 +24544,7 @@
         <v>1019</v>
       </c>
       <c r="F400" s="1" t="s">
-        <v>5940</v>
+        <v>5938</v>
       </c>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.6">
@@ -24546,7 +24558,7 @@
         <v>1021</v>
       </c>
       <c r="F401" s="1" t="s">
-        <v>5941</v>
+        <v>5939</v>
       </c>
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.6">
@@ -24560,7 +24572,7 @@
         <v>1023</v>
       </c>
       <c r="F402" s="1" t="s">
-        <v>5942</v>
+        <v>5940</v>
       </c>
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.6">
@@ -24574,21 +24586,21 @@
         <v>1025</v>
       </c>
       <c r="F403" s="1" t="s">
-        <v>5943</v>
+        <v>5941</v>
       </c>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.6">
       <c r="B404" s="1" t="s">
+        <v>5942</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>5942</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>5943</v>
+      </c>
+      <c r="F404" s="1" t="s">
         <v>5944</v>
-      </c>
-      <c r="C404" s="1" t="s">
-        <v>5944</v>
-      </c>
-      <c r="D404" s="1" t="s">
-        <v>5945</v>
-      </c>
-      <c r="F404" s="1" t="s">
-        <v>5946</v>
       </c>
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.6">
@@ -24602,7 +24614,7 @@
         <v>1027</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>5947</v>
+        <v>5945</v>
       </c>
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.6">
@@ -24616,7 +24628,7 @@
         <v>1029</v>
       </c>
       <c r="F406" s="1" t="s">
-        <v>5948</v>
+        <v>5946</v>
       </c>
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.6">
@@ -24630,7 +24642,7 @@
         <v>1031</v>
       </c>
       <c r="F407" s="1" t="s">
-        <v>5949</v>
+        <v>5947</v>
       </c>
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.6">
@@ -24644,7 +24656,7 @@
         <v>1033</v>
       </c>
       <c r="F408" s="1" t="s">
-        <v>5950</v>
+        <v>5948</v>
       </c>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.6">
@@ -24663,7 +24675,7 @@
         <v>1053</v>
       </c>
       <c r="F411" s="1" t="s">
-        <v>5951</v>
+        <v>5949</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.6">
@@ -24677,7 +24689,7 @@
         <v>1055</v>
       </c>
       <c r="F412" s="1" t="s">
-        <v>5952</v>
+        <v>5950</v>
       </c>
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.6">
@@ -24691,7 +24703,7 @@
         <v>1057</v>
       </c>
       <c r="F413" s="1" t="s">
-        <v>5953</v>
+        <v>5951</v>
       </c>
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.6">
@@ -24705,7 +24717,7 @@
         <v>1059</v>
       </c>
       <c r="F414" s="1" t="s">
-        <v>5954</v>
+        <v>5952</v>
       </c>
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.6">
@@ -24719,7 +24731,7 @@
         <v>1061</v>
       </c>
       <c r="F415" s="1" t="s">
-        <v>5955</v>
+        <v>5953</v>
       </c>
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.6">
@@ -24733,7 +24745,7 @@
         <v>1063</v>
       </c>
       <c r="F416" s="1" t="s">
-        <v>5956</v>
+        <v>5954</v>
       </c>
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.6">
@@ -24747,7 +24759,7 @@
         <v>1065</v>
       </c>
       <c r="F417" s="1" t="s">
-        <v>5957</v>
+        <v>5955</v>
       </c>
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.6">
@@ -24761,7 +24773,7 @@
         <v>1067</v>
       </c>
       <c r="F418" s="1" t="s">
-        <v>5958</v>
+        <v>5956</v>
       </c>
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.6">
@@ -24775,7 +24787,7 @@
         <v>1069</v>
       </c>
       <c r="F419" s="1" t="s">
-        <v>5959</v>
+        <v>5957</v>
       </c>
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.6">
@@ -24789,7 +24801,7 @@
         <v>1071</v>
       </c>
       <c r="F420" s="1" t="s">
-        <v>5960</v>
+        <v>5958</v>
       </c>
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.6">
@@ -24803,7 +24815,7 @@
         <v>1073</v>
       </c>
       <c r="F421" s="1" t="s">
-        <v>5961</v>
+        <v>5959</v>
       </c>
     </row>
     <row r="422" spans="1:6" x14ac:dyDescent="0.6">
@@ -24817,7 +24829,7 @@
         <v>1075</v>
       </c>
       <c r="F422" s="1" t="s">
-        <v>5962</v>
+        <v>5960</v>
       </c>
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.6">
@@ -24831,7 +24843,7 @@
         <v>1077</v>
       </c>
       <c r="F423" s="1" t="s">
-        <v>5963</v>
+        <v>5961</v>
       </c>
     </row>
     <row r="425" spans="1:6" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
Speed Master N3 Vocab.xlsx  ->  Part1 : 26 -> Word Corrected
</commit_message>
<xml_diff>
--- a/preparing/Speed Master N3 Vocab.xlsx
+++ b/preparing/Speed Master N3 Vocab.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7909" uniqueCount="7195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7911" uniqueCount="7199">
   <si>
     <t>yesterday</t>
   </si>
@@ -21610,6 +21610,19 @@
   <si>
     <t>Part1 : 26, 27, 28, 29, 30
 Myanmar Definition added.</t>
+  </si>
+  <si>
+    <t>入れ物</t>
+  </si>
+  <si>
+    <t>いれもの</t>
+  </si>
+  <si>
+    <t>container, case</t>
+  </si>
+  <si>
+    <t>Part1 : 26
+Word Corrected</t>
   </si>
 </sst>
 </file>
@@ -22018,7 +22031,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22196,11 +22209,19 @@
         <v>7194</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <v>43418</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5404</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>7198</v>
+      </c>
     </row>
     <row r="15" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
@@ -22254,8 +22275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1557"/>
   <sheetViews>
-    <sheetView topLeftCell="A1010" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1006" sqref="C1006"/>
+    <sheetView topLeftCell="A824" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B875" sqref="B875"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -42284,13 +42305,13 @@
         <v>815</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>2147</v>
+        <v>7195</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>2087</v>
+        <v>7196</v>
       </c>
       <c r="D875" s="1" t="s">
-        <v>2086</v>
+        <v>7197</v>
       </c>
       <c r="E875" s="7" t="s">
         <v>7081</v>
@@ -42300,7 +42321,7 @@
       </c>
       <c r="G875" s="1" t="str">
         <f t="shared" si="16"/>
-        <v>container ; ထည့်စရာ ; ထည့္စရာ</v>
+        <v>container, case ; ထည့်စရာ ; ထည့္စရာ</v>
       </c>
     </row>
     <row r="876" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -42308,13 +42329,13 @@
         <v>816</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>827</v>
+        <v>2147</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>827</v>
+        <v>2087</v>
       </c>
       <c r="D876" s="1" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="E876" s="7" t="s">
         <v>7082</v>
@@ -42324,7 +42345,7 @@
       </c>
       <c r="G876" s="1" t="str">
         <f t="shared" si="16"/>
-        <v>bottle ; ထည့်စရာခွက် ; ထည့္စရာခြက္</v>
+        <v>container ; ထည့်စရာခွက် ; ထည့္စရာခြက္</v>
       </c>
     </row>
     <row r="877" spans="1:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Speed Master N3 Vocab.xlsx -> Myanmar Definition updated -> Part1 : 28
</commit_message>
<xml_diff>
--- a/preparing/Speed Master N3 Vocab.xlsx
+++ b/preparing/Speed Master N3 Vocab.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7911" uniqueCount="7199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7913" uniqueCount="7202">
   <si>
     <t>yesterday</t>
   </si>
@@ -20921,18 +20921,12 @@
     <t>learning (する)</t>
   </si>
   <si>
-    <t>သင္ၾကားသည္</t>
-  </si>
-  <si>
     <t>လမ္းညႊန္ျပသျခင္း</t>
   </si>
   <si>
     <t>guidance (する)</t>
   </si>
   <si>
-    <t>သင္ယူသည္</t>
-  </si>
-  <si>
     <t>ဗဟုသုတ</t>
   </si>
   <si>
@@ -21413,13 +21407,7 @@
     <t>လေ့လာသင်ယူသည်</t>
   </si>
   <si>
-    <t>သင်ကြားသည်</t>
-  </si>
-  <si>
     <t>လမ်းညွှန်ပြသခြင်း</t>
-  </si>
-  <si>
-    <t>သင်ယူသည်</t>
   </si>
   <si>
     <t>ကျောင်းသွားကျောင်းပြန်လုပ်ခြင်း</t>
@@ -21623,6 +21611,28 @@
   <si>
     <t>Part1 : 26
 Word Corrected</t>
+  </si>
+  <si>
+    <t>သင်ယူရရှိသည်</t>
+  </si>
+  <si>
+    <t>သင္ယူရရွိသည္</t>
+  </si>
+  <si>
+    <t>သင်ကြားပေးခံရသည်</t>
+  </si>
+  <si>
+    <t>သင္ၾကားေပးခံရသည္</t>
+  </si>
+  <si>
+    <t>သင်ကြားပေးသည်</t>
+  </si>
+  <si>
+    <t>သင္ၾကားေပးသည္</t>
+  </si>
+  <si>
+    <t>Part1 : 28
+Myanmar Definition updated.</t>
   </si>
 </sst>
 </file>
@@ -22030,8 +22040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22206,7 +22216,7 @@
         <v>5404</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>7194</v>
+        <v>7190</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -22220,14 +22230,22 @@
         <v>5404</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>7198</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+        <v>7194</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43424</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5404</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>7201</v>
+      </c>
     </row>
     <row r="16" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -22275,8 +22293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1557"/>
   <sheetViews>
-    <sheetView topLeftCell="A824" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B875" sqref="B875"/>
+    <sheetView topLeftCell="A930" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C934" sqref="C934"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -41213,7 +41231,7 @@
         <v>2001</v>
       </c>
       <c r="E829" s="7" t="s">
-        <v>7040</v>
+        <v>7038</v>
       </c>
       <c r="F829" s="1" t="s">
         <v>6860</v>
@@ -41237,7 +41255,7 @@
         <v>2003</v>
       </c>
       <c r="E830" s="7" t="s">
-        <v>7041</v>
+        <v>7039</v>
       </c>
       <c r="F830" s="1" t="s">
         <v>6861</v>
@@ -41261,7 +41279,7 @@
         <v>2005</v>
       </c>
       <c r="E831" s="7" t="s">
-        <v>7042</v>
+        <v>7040</v>
       </c>
       <c r="F831" s="1" t="s">
         <v>6862</v>
@@ -41285,7 +41303,7 @@
         <v>2007</v>
       </c>
       <c r="E832" s="7" t="s">
-        <v>7043</v>
+        <v>7041</v>
       </c>
       <c r="F832" s="1" t="s">
         <v>6863</v>
@@ -41306,7 +41324,7 @@
         <v>6869</v>
       </c>
       <c r="E833" s="7" t="s">
-        <v>7044</v>
+        <v>7042</v>
       </c>
       <c r="F833" s="1" t="s">
         <v>6864</v>
@@ -41330,7 +41348,7 @@
         <v>2009</v>
       </c>
       <c r="E834" s="7" t="s">
-        <v>7045</v>
+        <v>7043</v>
       </c>
       <c r="F834" s="1" t="s">
         <v>6865</v>
@@ -41354,7 +41372,7 @@
         <v>2011</v>
       </c>
       <c r="E835" s="7" t="s">
-        <v>7046</v>
+        <v>7044</v>
       </c>
       <c r="F835" s="1" t="s">
         <v>6866</v>
@@ -41378,7 +41396,7 @@
         <v>2013</v>
       </c>
       <c r="E836" s="7" t="s">
-        <v>7047</v>
+        <v>7045</v>
       </c>
       <c r="F836" s="1" t="s">
         <v>6870</v>
@@ -41402,7 +41420,7 @@
         <v>2015</v>
       </c>
       <c r="E837" s="7" t="s">
-        <v>7048</v>
+        <v>7046</v>
       </c>
       <c r="F837" s="1" t="s">
         <v>6871</v>
@@ -41426,7 +41444,7 @@
         <v>2017</v>
       </c>
       <c r="E838" s="7" t="s">
-        <v>7049</v>
+        <v>7047</v>
       </c>
       <c r="F838" s="1" t="s">
         <v>6872</v>
@@ -41450,7 +41468,7 @@
         <v>2019</v>
       </c>
       <c r="E839" s="7" t="s">
-        <v>7050</v>
+        <v>7048</v>
       </c>
       <c r="F839" s="1" t="s">
         <v>6873</v>
@@ -41474,7 +41492,7 @@
         <v>2021</v>
       </c>
       <c r="E840" s="7" t="s">
-        <v>7051</v>
+        <v>7049</v>
       </c>
       <c r="F840" s="1" t="s">
         <v>6874</v>
@@ -41498,7 +41516,7 @@
         <v>6876</v>
       </c>
       <c r="E841" s="7" t="s">
-        <v>7052</v>
+        <v>7050</v>
       </c>
       <c r="F841" s="1" t="s">
         <v>6875</v>
@@ -41522,7 +41540,7 @@
         <v>2024</v>
       </c>
       <c r="E842" s="7" t="s">
-        <v>7053</v>
+        <v>7051</v>
       </c>
       <c r="F842" s="1" t="s">
         <v>6877</v>
@@ -41546,7 +41564,7 @@
         <v>2025</v>
       </c>
       <c r="E843" s="7" t="s">
-        <v>7054</v>
+        <v>7052</v>
       </c>
       <c r="F843" s="1" t="s">
         <v>6878</v>
@@ -41570,7 +41588,7 @@
         <v>6880</v>
       </c>
       <c r="E844" s="7" t="s">
-        <v>7055</v>
+        <v>7053</v>
       </c>
       <c r="F844" s="1" t="s">
         <v>6879</v>
@@ -41594,7 +41612,7 @@
         <v>2028</v>
       </c>
       <c r="E845" s="7" t="s">
-        <v>7056</v>
+        <v>7054</v>
       </c>
       <c r="F845" s="1" t="s">
         <v>6881</v>
@@ -41618,7 +41636,7 @@
         <v>2030</v>
       </c>
       <c r="E846" s="7" t="s">
-        <v>7057</v>
+        <v>7055</v>
       </c>
       <c r="F846" s="1" t="s">
         <v>6882</v>
@@ -41666,7 +41684,7 @@
         <v>2034</v>
       </c>
       <c r="E848" s="7" t="s">
-        <v>7058</v>
+        <v>7056</v>
       </c>
       <c r="F848" s="1" t="s">
         <v>6884</v>
@@ -41690,7 +41708,7 @@
         <v>2036</v>
       </c>
       <c r="E849" s="7" t="s">
-        <v>7059</v>
+        <v>7057</v>
       </c>
       <c r="F849" s="1" t="s">
         <v>6885</v>
@@ -41714,7 +41732,7 @@
         <v>2038</v>
       </c>
       <c r="E850" s="7" t="s">
-        <v>7060</v>
+        <v>7058</v>
       </c>
       <c r="F850" s="1" t="s">
         <v>6886</v>
@@ -41738,7 +41756,7 @@
         <v>2040</v>
       </c>
       <c r="E851" s="7" t="s">
-        <v>7061</v>
+        <v>7059</v>
       </c>
       <c r="F851" s="1" t="s">
         <v>6887</v>
@@ -41762,7 +41780,7 @@
         <v>6890</v>
       </c>
       <c r="E852" s="7" t="s">
-        <v>7062</v>
+        <v>7060</v>
       </c>
       <c r="F852" s="1" t="s">
         <v>6888</v>
@@ -41786,7 +41804,7 @@
         <v>2043</v>
       </c>
       <c r="E853" s="7" t="s">
-        <v>7062</v>
+        <v>7060</v>
       </c>
       <c r="F853" s="1" t="s">
         <v>6888</v>
@@ -41810,7 +41828,7 @@
         <v>2045</v>
       </c>
       <c r="E854" s="7" t="s">
-        <v>7063</v>
+        <v>7061</v>
       </c>
       <c r="F854" s="1" t="s">
         <v>6889</v>
@@ -41858,7 +41876,7 @@
         <v>2049</v>
       </c>
       <c r="E856" s="7" t="s">
-        <v>7064</v>
+        <v>7062</v>
       </c>
       <c r="F856" s="1" t="s">
         <v>6891</v>
@@ -41882,7 +41900,7 @@
         <v>2051</v>
       </c>
       <c r="E857" s="7" t="s">
-        <v>7065</v>
+        <v>7063</v>
       </c>
       <c r="F857" s="1" t="s">
         <v>6892</v>
@@ -41906,7 +41924,7 @@
         <v>2053</v>
       </c>
       <c r="E858" s="7" t="s">
-        <v>7066</v>
+        <v>7064</v>
       </c>
       <c r="F858" s="1" t="s">
         <v>6893</v>
@@ -41930,7 +41948,7 @@
         <v>2055</v>
       </c>
       <c r="E859" s="7" t="s">
-        <v>7067</v>
+        <v>7065</v>
       </c>
       <c r="F859" s="1" t="s">
         <v>6894</v>
@@ -41954,7 +41972,7 @@
         <v>2057</v>
       </c>
       <c r="E860" s="7" t="s">
-        <v>7068</v>
+        <v>7066</v>
       </c>
       <c r="F860" s="1" t="s">
         <v>6895</v>
@@ -41978,7 +41996,7 @@
         <v>2059</v>
       </c>
       <c r="E861" s="7" t="s">
-        <v>7069</v>
+        <v>7067</v>
       </c>
       <c r="F861" s="1" t="s">
         <v>6896</v>
@@ -42002,7 +42020,7 @@
         <v>2061</v>
       </c>
       <c r="E862" s="7" t="s">
-        <v>7070</v>
+        <v>7068</v>
       </c>
       <c r="F862" s="1" t="s">
         <v>6897</v>
@@ -42026,7 +42044,7 @@
         <v>2063</v>
       </c>
       <c r="E863" s="7" t="s">
-        <v>7071</v>
+        <v>7069</v>
       </c>
       <c r="F863" s="1" t="s">
         <v>6898</v>
@@ -42050,7 +42068,7 @@
         <v>6899</v>
       </c>
       <c r="E864" s="7" t="s">
-        <v>7071</v>
+        <v>7069</v>
       </c>
       <c r="F864" s="1" t="s">
         <v>6898</v>
@@ -42074,7 +42092,7 @@
         <v>2066</v>
       </c>
       <c r="E865" s="7" t="s">
-        <v>7072</v>
+        <v>7070</v>
       </c>
       <c r="F865" s="1" t="s">
         <v>6900</v>
@@ -42098,7 +42116,7 @@
         <v>2068</v>
       </c>
       <c r="E866" s="7" t="s">
-        <v>7073</v>
+        <v>7071</v>
       </c>
       <c r="F866" s="1" t="s">
         <v>6901</v>
@@ -42122,7 +42140,7 @@
         <v>2070</v>
       </c>
       <c r="E867" s="7" t="s">
-        <v>7074</v>
+        <v>7072</v>
       </c>
       <c r="F867" s="1" t="s">
         <v>6902</v>
@@ -42146,7 +42164,7 @@
         <v>2072</v>
       </c>
       <c r="E868" s="7" t="s">
-        <v>7075</v>
+        <v>7073</v>
       </c>
       <c r="F868" s="1" t="s">
         <v>6903</v>
@@ -42170,7 +42188,7 @@
         <v>2074</v>
       </c>
       <c r="E869" s="7" t="s">
-        <v>7076</v>
+        <v>7074</v>
       </c>
       <c r="F869" s="1" t="s">
         <v>6904</v>
@@ -42194,7 +42212,7 @@
         <v>2076</v>
       </c>
       <c r="E870" s="7" t="s">
-        <v>7077</v>
+        <v>7075</v>
       </c>
       <c r="F870" s="1" t="s">
         <v>6905</v>
@@ -42218,7 +42236,7 @@
         <v>2078</v>
       </c>
       <c r="E871" s="7" t="s">
-        <v>7078</v>
+        <v>7076</v>
       </c>
       <c r="F871" s="1" t="s">
         <v>6906</v>
@@ -42242,7 +42260,7 @@
         <v>2080</v>
       </c>
       <c r="E872" s="7" t="s">
-        <v>7079</v>
+        <v>7077</v>
       </c>
       <c r="F872" s="1" t="s">
         <v>6907</v>
@@ -42266,7 +42284,7 @@
         <v>2082</v>
       </c>
       <c r="E873" s="7" t="s">
-        <v>7080</v>
+        <v>7078</v>
       </c>
       <c r="F873" s="1" t="s">
         <v>6908</v>
@@ -42305,16 +42323,16 @@
         <v>815</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>7195</v>
+        <v>7191</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>7196</v>
+        <v>7192</v>
       </c>
       <c r="D875" s="1" t="s">
-        <v>7197</v>
+        <v>7193</v>
       </c>
       <c r="E875" s="7" t="s">
-        <v>7081</v>
+        <v>7079</v>
       </c>
       <c r="F875" s="1" t="s">
         <v>6910</v>
@@ -42338,7 +42356,7 @@
         <v>2086</v>
       </c>
       <c r="E876" s="7" t="s">
-        <v>7082</v>
+        <v>7080</v>
       </c>
       <c r="F876" s="1" t="s">
         <v>6911</v>
@@ -42362,7 +42380,7 @@
         <v>2089</v>
       </c>
       <c r="E877" s="7" t="s">
-        <v>7083</v>
+        <v>7081</v>
       </c>
       <c r="F877" s="1" t="s">
         <v>6912</v>
@@ -42386,7 +42404,7 @@
         <v>6913</v>
       </c>
       <c r="E878" s="7" t="s">
-        <v>7084</v>
+        <v>7082</v>
       </c>
       <c r="F878" s="1" t="s">
         <v>6914</v>
@@ -42410,7 +42428,7 @@
         <v>2093</v>
       </c>
       <c r="E879" s="7" t="s">
-        <v>7085</v>
+        <v>7083</v>
       </c>
       <c r="F879" s="1" t="s">
         <v>6915</v>
@@ -42434,7 +42452,7 @@
         <v>2088</v>
       </c>
       <c r="E880" s="1" t="s">
-        <v>7086</v>
+        <v>7084</v>
       </c>
       <c r="F880" s="1" t="s">
         <v>6916</v>
@@ -42455,7 +42473,7 @@
         <v>2095</v>
       </c>
       <c r="E881" s="7" t="s">
-        <v>7087</v>
+        <v>7085</v>
       </c>
       <c r="F881" s="1" t="s">
         <v>6918</v>
@@ -42479,7 +42497,7 @@
         <v>2097</v>
       </c>
       <c r="E882" s="7" t="s">
-        <v>7088</v>
+        <v>7086</v>
       </c>
       <c r="F882" s="1" t="s">
         <v>6917</v>
@@ -42503,7 +42521,7 @@
         <v>2099</v>
       </c>
       <c r="E883" s="7" t="s">
-        <v>7089</v>
+        <v>7087</v>
       </c>
       <c r="F883" s="1" t="s">
         <v>6919</v>
@@ -42527,7 +42545,7 @@
         <v>2101</v>
       </c>
       <c r="E884" s="7" t="s">
-        <v>7090</v>
+        <v>7088</v>
       </c>
       <c r="F884" s="1" t="s">
         <v>6920</v>
@@ -42551,7 +42569,7 @@
         <v>2103</v>
       </c>
       <c r="E885" s="7" t="s">
-        <v>7091</v>
+        <v>7089</v>
       </c>
       <c r="F885" s="1" t="s">
         <v>6921</v>
@@ -42575,7 +42593,7 @@
         <v>2105</v>
       </c>
       <c r="E886" s="7" t="s">
-        <v>7092</v>
+        <v>7090</v>
       </c>
       <c r="F886" s="1" t="s">
         <v>6922</v>
@@ -42599,7 +42617,7 @@
         <v>2107</v>
       </c>
       <c r="E887" s="7" t="s">
-        <v>7093</v>
+        <v>7091</v>
       </c>
       <c r="F887" s="1" t="s">
         <v>6923</v>
@@ -42623,7 +42641,7 @@
         <v>2109</v>
       </c>
       <c r="E888" s="7" t="s">
-        <v>7094</v>
+        <v>7092</v>
       </c>
       <c r="F888" s="1" t="s">
         <v>6924</v>
@@ -42647,7 +42665,7 @@
         <v>6004</v>
       </c>
       <c r="E889" s="7" t="s">
-        <v>7095</v>
+        <v>7093</v>
       </c>
       <c r="F889" s="1" t="s">
         <v>6925</v>
@@ -42671,7 +42689,7 @@
         <v>1954</v>
       </c>
       <c r="E890" s="7" t="s">
-        <v>7096</v>
+        <v>7094</v>
       </c>
       <c r="F890" s="1" t="s">
         <v>6926</v>
@@ -42695,7 +42713,7 @@
         <v>6927</v>
       </c>
       <c r="E891" s="7" t="s">
-        <v>7097</v>
+        <v>7095</v>
       </c>
       <c r="F891" s="1" t="s">
         <v>6928</v>
@@ -42719,7 +42737,7 @@
         <v>2112</v>
       </c>
       <c r="E892" s="7" t="s">
-        <v>7098</v>
+        <v>7096</v>
       </c>
       <c r="F892" s="1" t="s">
         <v>6929</v>
@@ -42743,7 +42761,7 @@
         <v>2114</v>
       </c>
       <c r="E893" s="7" t="s">
-        <v>7099</v>
+        <v>7097</v>
       </c>
       <c r="F893" s="1" t="s">
         <v>6930</v>
@@ -42767,7 +42785,7 @@
         <v>2116</v>
       </c>
       <c r="E894" s="7" t="s">
-        <v>7100</v>
+        <v>7098</v>
       </c>
       <c r="F894" s="1" t="s">
         <v>6931</v>
@@ -42791,7 +42809,7 @@
         <v>2118</v>
       </c>
       <c r="E895" s="7" t="s">
-        <v>7101</v>
+        <v>7099</v>
       </c>
       <c r="F895" s="1" t="s">
         <v>6932</v>
@@ -42815,7 +42833,7 @@
         <v>2120</v>
       </c>
       <c r="E896" s="7" t="s">
-        <v>7102</v>
+        <v>7100</v>
       </c>
       <c r="F896" s="1" t="s">
         <v>6933</v>
@@ -42839,7 +42857,7 @@
         <v>2122</v>
       </c>
       <c r="E897" s="7" t="s">
-        <v>7103</v>
+        <v>7101</v>
       </c>
       <c r="F897" s="1" t="s">
         <v>6934</v>
@@ -42878,7 +42896,7 @@
         <v>2155</v>
       </c>
       <c r="E900" s="7" t="s">
-        <v>7104</v>
+        <v>7102</v>
       </c>
       <c r="F900" s="1" t="s">
         <v>6935</v>
@@ -42902,7 +42920,7 @@
         <v>2157</v>
       </c>
       <c r="E901" s="7" t="s">
-        <v>7104</v>
+        <v>7102</v>
       </c>
       <c r="F901" s="1" t="s">
         <v>6935</v>
@@ -42950,7 +42968,7 @@
         <v>2161</v>
       </c>
       <c r="E903" s="7" t="s">
-        <v>7105</v>
+        <v>7103</v>
       </c>
       <c r="F903" s="1" t="s">
         <v>6936</v>
@@ -42998,7 +43016,7 @@
         <v>2164</v>
       </c>
       <c r="E905" s="7" t="s">
-        <v>7106</v>
+        <v>7104</v>
       </c>
       <c r="F905" s="1" t="s">
         <v>6937</v>
@@ -43022,7 +43040,7 @@
         <v>2166</v>
       </c>
       <c r="E906" s="7" t="s">
-        <v>7107</v>
+        <v>7105</v>
       </c>
       <c r="F906" s="1" t="s">
         <v>6938</v>
@@ -43046,7 +43064,7 @@
         <v>2168</v>
       </c>
       <c r="E907" s="7" t="s">
-        <v>7108</v>
+        <v>7106</v>
       </c>
       <c r="F907" s="1" t="s">
         <v>6939</v>
@@ -43070,7 +43088,7 @@
         <v>2170</v>
       </c>
       <c r="E908" s="7" t="s">
-        <v>7109</v>
+        <v>7107</v>
       </c>
       <c r="F908" s="1" t="s">
         <v>6940</v>
@@ -43094,7 +43112,7 @@
         <v>2172</v>
       </c>
       <c r="E909" s="7" t="s">
-        <v>7110</v>
+        <v>7108</v>
       </c>
       <c r="F909" s="1" t="s">
         <v>6941</v>
@@ -43142,7 +43160,7 @@
         <v>2176</v>
       </c>
       <c r="E911" s="7" t="s">
-        <v>7111</v>
+        <v>7109</v>
       </c>
       <c r="F911" s="1" t="s">
         <v>6942</v>
@@ -43190,7 +43208,7 @@
         <v>2180</v>
       </c>
       <c r="E913" s="7" t="s">
-        <v>7112</v>
+        <v>7110</v>
       </c>
       <c r="F913" s="1" t="s">
         <v>6943</v>
@@ -43214,7 +43232,7 @@
         <v>2182</v>
       </c>
       <c r="E914" s="7" t="s">
-        <v>7113</v>
+        <v>7111</v>
       </c>
       <c r="F914" s="1" t="s">
         <v>6944</v>
@@ -43238,7 +43256,7 @@
         <v>2184</v>
       </c>
       <c r="E915" s="7" t="s">
-        <v>7114</v>
+        <v>7112</v>
       </c>
       <c r="F915" s="1" t="s">
         <v>6945</v>
@@ -43262,7 +43280,7 @@
         <v>2186</v>
       </c>
       <c r="E916" s="7" t="s">
-        <v>7115</v>
+        <v>7113</v>
       </c>
       <c r="F916" s="1" t="s">
         <v>6946</v>
@@ -43286,7 +43304,7 @@
         <v>2187</v>
       </c>
       <c r="E917" s="7" t="s">
-        <v>7116</v>
+        <v>7114</v>
       </c>
       <c r="F917" s="1" t="s">
         <v>6947</v>
@@ -43310,7 +43328,7 @@
         <v>2189</v>
       </c>
       <c r="E918" s="7" t="s">
-        <v>7117</v>
+        <v>7115</v>
       </c>
       <c r="F918" s="1" t="s">
         <v>6948</v>
@@ -43334,7 +43352,7 @@
         <v>2191</v>
       </c>
       <c r="E919" s="7" t="s">
-        <v>7118</v>
+        <v>7116</v>
       </c>
       <c r="F919" s="1" t="s">
         <v>6949</v>
@@ -43382,7 +43400,7 @@
         <v>2195</v>
       </c>
       <c r="E921" s="7" t="s">
-        <v>7119</v>
+        <v>7117</v>
       </c>
       <c r="F921" s="1" t="s">
         <v>6951</v>
@@ -43430,7 +43448,7 @@
         <v>2199</v>
       </c>
       <c r="E923" s="7" t="s">
-        <v>7120</v>
+        <v>7118</v>
       </c>
       <c r="F923" s="1" t="s">
         <v>6953</v>
@@ -43454,7 +43472,7 @@
         <v>2201</v>
       </c>
       <c r="E924" s="7" t="s">
-        <v>7121</v>
+        <v>7119</v>
       </c>
       <c r="F924" s="1" t="s">
         <v>6954</v>
@@ -43478,7 +43496,7 @@
         <v>2203</v>
       </c>
       <c r="E925" s="7" t="s">
-        <v>7122</v>
+        <v>7120</v>
       </c>
       <c r="F925" s="1" t="s">
         <v>6955</v>
@@ -43502,7 +43520,7 @@
         <v>2205</v>
       </c>
       <c r="E926" s="7" t="s">
-        <v>7123</v>
+        <v>7121</v>
       </c>
       <c r="F926" s="1" t="s">
         <v>6956</v>
@@ -43550,7 +43568,7 @@
         <v>2209</v>
       </c>
       <c r="E928" s="7" t="s">
-        <v>7124</v>
+        <v>7122</v>
       </c>
       <c r="F928" s="1" t="s">
         <v>6958</v>
@@ -43574,7 +43592,7 @@
         <v>2211</v>
       </c>
       <c r="E929" s="7" t="s">
-        <v>7125</v>
+        <v>7123</v>
       </c>
       <c r="F929" s="1" t="s">
         <v>6959</v>
@@ -43598,7 +43616,7 @@
         <v>6961</v>
       </c>
       <c r="E930" s="7" t="s">
-        <v>7126</v>
+        <v>7124</v>
       </c>
       <c r="F930" s="1" t="s">
         <v>6960</v>
@@ -43637,7 +43655,7 @@
         <v>6964</v>
       </c>
       <c r="E933" s="7" t="s">
-        <v>7127</v>
+        <v>7125</v>
       </c>
       <c r="F933" s="1" t="s">
         <v>6962</v>
@@ -43661,7 +43679,7 @@
         <v>2239</v>
       </c>
       <c r="E934" s="7" t="s">
-        <v>7128</v>
+        <v>7126</v>
       </c>
       <c r="F934" s="1" t="s">
         <v>6963</v>
@@ -43685,14 +43703,14 @@
         <v>2241</v>
       </c>
       <c r="E935" s="7" t="s">
-        <v>7129</v>
+        <v>7195</v>
       </c>
       <c r="F935" s="1" t="s">
-        <v>6965</v>
+        <v>7196</v>
       </c>
       <c r="G935" s="1" t="str">
         <f t="shared" si="17"/>
-        <v>to learn, to take lessons in ; သင်ကြားသည် ; သင္ၾကားသည္</v>
+        <v>to learn, to take lessons in ; သင်ယူရရှိသည် ; သင္ယူရရွိသည္</v>
       </c>
     </row>
     <row r="936" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -43706,13 +43724,13 @@
         <v>2244</v>
       </c>
       <c r="D936" s="1" t="s">
-        <v>6967</v>
+        <v>6966</v>
       </c>
       <c r="E936" s="7" t="s">
-        <v>7130</v>
+        <v>7127</v>
       </c>
       <c r="F936" s="1" t="s">
-        <v>6966</v>
+        <v>6965</v>
       </c>
       <c r="G936" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43733,14 +43751,14 @@
         <v>2245</v>
       </c>
       <c r="E937" s="7" t="s">
-        <v>7131</v>
+        <v>7197</v>
       </c>
       <c r="F937" s="1" t="s">
-        <v>6968</v>
+        <v>7198</v>
       </c>
       <c r="G937" s="1" t="str">
         <f t="shared" si="17"/>
-        <v>to be taught ; သင်ယူသည် ; သင္ယူသည္</v>
+        <v>to be taught ; သင်ကြားပေးခံရသည် ; သင္ၾကားေပးခံရသည္</v>
       </c>
     </row>
     <row r="938" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -43748,7 +43766,7 @@
         <v>873</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>7193</v>
+        <v>7189</v>
       </c>
       <c r="C938" s="1" t="s">
         <v>2248</v>
@@ -43757,14 +43775,14 @@
         <v>2247</v>
       </c>
       <c r="E938" s="7" t="s">
-        <v>7129</v>
+        <v>7199</v>
       </c>
       <c r="F938" s="1" t="s">
-        <v>6965</v>
+        <v>7200</v>
       </c>
       <c r="G938" s="1" t="str">
         <f t="shared" si="17"/>
-        <v>to teach ; သင်ကြားသည် ; သင္ၾကားသည္</v>
+        <v>to teach ; သင်ကြားပေးသည် ; သင္ၾကားေပးသည္</v>
       </c>
     </row>
     <row r="939" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -43781,10 +43799,10 @@
         <v>2249</v>
       </c>
       <c r="E939" s="7" t="s">
-        <v>6969</v>
+        <v>6967</v>
       </c>
       <c r="F939" s="1" t="s">
-        <v>6969</v>
+        <v>6967</v>
       </c>
       <c r="G939" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43802,13 +43820,13 @@
         <v>2251</v>
       </c>
       <c r="D940" s="1" t="s">
-        <v>6971</v>
+        <v>6969</v>
       </c>
       <c r="E940" s="7" t="s">
-        <v>7132</v>
+        <v>7128</v>
       </c>
       <c r="F940" s="1" t="s">
-        <v>6970</v>
+        <v>6968</v>
       </c>
       <c r="G940" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43829,10 +43847,10 @@
         <v>2252</v>
       </c>
       <c r="E941" s="7" t="s">
-        <v>7133</v>
+        <v>7129</v>
       </c>
       <c r="F941" s="1" t="s">
-        <v>6972</v>
+        <v>6970</v>
       </c>
       <c r="G941" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43853,10 +43871,10 @@
         <v>2254</v>
       </c>
       <c r="E942" s="7" t="s">
-        <v>7134</v>
+        <v>7130</v>
       </c>
       <c r="F942" s="1" t="s">
-        <v>6973</v>
+        <v>6971</v>
       </c>
       <c r="G942" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43877,10 +43895,10 @@
         <v>1011</v>
       </c>
       <c r="E943" s="7" t="s">
-        <v>7135</v>
+        <v>7131</v>
       </c>
       <c r="F943" s="1" t="s">
-        <v>6974</v>
+        <v>6972</v>
       </c>
       <c r="G943" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43901,10 +43919,10 @@
         <v>2257</v>
       </c>
       <c r="E944" s="7" t="s">
-        <v>7136</v>
+        <v>7132</v>
       </c>
       <c r="F944" s="1" t="s">
-        <v>6975</v>
+        <v>6973</v>
       </c>
       <c r="G944" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43925,10 +43943,10 @@
         <v>2259</v>
       </c>
       <c r="E945" s="7" t="s">
-        <v>7137</v>
+        <v>7133</v>
       </c>
       <c r="F945" s="1" t="s">
-        <v>6976</v>
+        <v>6974</v>
       </c>
       <c r="G945" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43949,10 +43967,10 @@
         <v>2261</v>
       </c>
       <c r="E946" s="7" t="s">
-        <v>7138</v>
+        <v>7134</v>
       </c>
       <c r="F946" s="1" t="s">
-        <v>6977</v>
+        <v>6975</v>
       </c>
       <c r="G946" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43973,10 +43991,10 @@
         <v>2263</v>
       </c>
       <c r="E947" s="7" t="s">
-        <v>7139</v>
+        <v>7135</v>
       </c>
       <c r="F947" s="1" t="s">
-        <v>6978</v>
+        <v>6976</v>
       </c>
       <c r="G947" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43997,10 +44015,10 @@
         <v>2265</v>
       </c>
       <c r="E948" s="7" t="s">
-        <v>7140</v>
+        <v>7136</v>
       </c>
       <c r="F948" s="1" t="s">
-        <v>6979</v>
+        <v>6977</v>
       </c>
       <c r="G948" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44021,10 +44039,10 @@
         <v>2267</v>
       </c>
       <c r="E949" s="7" t="s">
-        <v>7141</v>
+        <v>7137</v>
       </c>
       <c r="F949" s="1" t="s">
-        <v>6980</v>
+        <v>6978</v>
       </c>
       <c r="G949" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44045,10 +44063,10 @@
         <v>2269</v>
       </c>
       <c r="E950" s="7" t="s">
-        <v>7142</v>
+        <v>7138</v>
       </c>
       <c r="F950" s="1" t="s">
-        <v>6981</v>
+        <v>6979</v>
       </c>
       <c r="G950" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44069,10 +44087,10 @@
         <v>2271</v>
       </c>
       <c r="E951" s="7" t="s">
-        <v>7143</v>
+        <v>7139</v>
       </c>
       <c r="F951" s="1" t="s">
-        <v>6982</v>
+        <v>6980</v>
       </c>
       <c r="G951" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44093,10 +44111,10 @@
         <v>2273</v>
       </c>
       <c r="E952" s="7" t="s">
-        <v>7144</v>
+        <v>7140</v>
       </c>
       <c r="F952" s="1" t="s">
-        <v>6983</v>
+        <v>6981</v>
       </c>
       <c r="G952" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44132,19 +44150,19 @@
         <v>889</v>
       </c>
       <c r="B954" s="1" t="s">
+        <v>6982</v>
+      </c>
+      <c r="C954" s="1" t="s">
+        <v>6983</v>
+      </c>
+      <c r="D954" s="1" t="s">
         <v>6984</v>
       </c>
-      <c r="C954" s="1" t="s">
+      <c r="E954" s="7" t="s">
+        <v>7141</v>
+      </c>
+      <c r="F954" s="1" t="s">
         <v>6985</v>
-      </c>
-      <c r="D954" s="1" t="s">
-        <v>6986</v>
-      </c>
-      <c r="E954" s="7" t="s">
-        <v>7145</v>
-      </c>
-      <c r="F954" s="1" t="s">
-        <v>6987</v>
       </c>
       <c r="G954" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44165,10 +44183,10 @@
         <v>2277</v>
       </c>
       <c r="E955" s="7" t="s">
-        <v>7146</v>
+        <v>7142</v>
       </c>
       <c r="F955" s="1" t="s">
-        <v>6988</v>
+        <v>6986</v>
       </c>
       <c r="G955" s="1" t="str">
         <f t="shared" si="17"/>
@@ -44189,10 +44207,10 @@
         <v>2279</v>
       </c>
       <c r="E956" s="7" t="s">
-        <v>7147</v>
+        <v>7143</v>
       </c>
       <c r="F956" s="1" t="s">
-        <v>6989</v>
+        <v>6987</v>
       </c>
       <c r="G956" s="1" t="str">
         <f t="shared" ref="G956:G1011" si="18">CONCATENATE(D956, " ; ",E956," ; ",F956)</f>
@@ -44213,10 +44231,10 @@
         <v>2281</v>
       </c>
       <c r="E957" s="7" t="s">
-        <v>7135</v>
+        <v>7131</v>
       </c>
       <c r="F957" s="1" t="s">
-        <v>6974</v>
+        <v>6972</v>
       </c>
       <c r="G957" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44237,10 +44255,10 @@
         <v>2283</v>
       </c>
       <c r="E958" s="7" t="s">
-        <v>7148</v>
+        <v>7144</v>
       </c>
       <c r="F958" s="1" t="s">
-        <v>6990</v>
+        <v>6988</v>
       </c>
       <c r="G958" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44261,10 +44279,10 @@
         <v>2285</v>
       </c>
       <c r="E959" s="7" t="s">
-        <v>7149</v>
+        <v>7145</v>
       </c>
       <c r="F959" s="1" t="s">
-        <v>6991</v>
+        <v>6989</v>
       </c>
       <c r="G959" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44300,10 +44318,10 @@
         <v>2310</v>
       </c>
       <c r="E962" s="7" t="s">
-        <v>7150</v>
+        <v>7146</v>
       </c>
       <c r="F962" s="1" t="s">
-        <v>6992</v>
+        <v>6990</v>
       </c>
       <c r="G962" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44324,10 +44342,10 @@
         <v>2312</v>
       </c>
       <c r="E963" s="7" t="s">
-        <v>7151</v>
+        <v>7147</v>
       </c>
       <c r="F963" s="1" t="s">
-        <v>6993</v>
+        <v>6991</v>
       </c>
       <c r="G963" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44348,10 +44366,10 @@
         <v>2314</v>
       </c>
       <c r="E964" s="7" t="s">
-        <v>7152</v>
+        <v>7148</v>
       </c>
       <c r="F964" s="1" t="s">
-        <v>6994</v>
+        <v>6992</v>
       </c>
       <c r="G964" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44372,10 +44390,10 @@
         <v>2316</v>
       </c>
       <c r="E965" s="7" t="s">
-        <v>7153</v>
+        <v>7149</v>
       </c>
       <c r="F965" s="1" t="s">
-        <v>6995</v>
+        <v>6993</v>
       </c>
       <c r="G965" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44396,10 +44414,10 @@
         <v>2318</v>
       </c>
       <c r="E966" s="7" t="s">
-        <v>7154</v>
+        <v>7150</v>
       </c>
       <c r="F966" s="1" t="s">
-        <v>6996</v>
+        <v>6994</v>
       </c>
       <c r="G966" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44420,10 +44438,10 @@
         <v>2320</v>
       </c>
       <c r="E967" s="7" t="s">
-        <v>7155</v>
+        <v>7151</v>
       </c>
       <c r="F967" s="1" t="s">
-        <v>6997</v>
+        <v>6995</v>
       </c>
       <c r="G967" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44444,10 +44462,10 @@
         <v>2322</v>
       </c>
       <c r="E968" s="7" t="s">
-        <v>7156</v>
+        <v>7152</v>
       </c>
       <c r="F968" s="1" t="s">
-        <v>6998</v>
+        <v>6996</v>
       </c>
       <c r="G968" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44468,10 +44486,10 @@
         <v>2324</v>
       </c>
       <c r="E969" s="7" t="s">
-        <v>7157</v>
+        <v>7153</v>
       </c>
       <c r="F969" s="1" t="s">
-        <v>6999</v>
+        <v>6997</v>
       </c>
       <c r="G969" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44492,10 +44510,10 @@
         <v>2326</v>
       </c>
       <c r="E970" s="7" t="s">
-        <v>7000</v>
+        <v>6998</v>
       </c>
       <c r="F970" s="1" t="s">
-        <v>7000</v>
+        <v>6998</v>
       </c>
       <c r="G970" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44516,10 +44534,10 @@
         <v>2281</v>
       </c>
       <c r="E971" s="10" t="s">
-        <v>7135</v>
+        <v>7131</v>
       </c>
       <c r="F971" s="8" t="s">
-        <v>6974</v>
+        <v>6972</v>
       </c>
       <c r="G971" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44540,10 +44558,10 @@
         <v>2328</v>
       </c>
       <c r="E972" s="7" t="s">
-        <v>7158</v>
+        <v>7154</v>
       </c>
       <c r="F972" s="1" t="s">
-        <v>7001</v>
+        <v>6999</v>
       </c>
       <c r="G972" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44564,10 +44582,10 @@
         <v>2330</v>
       </c>
       <c r="E973" s="7" t="s">
-        <v>7159</v>
+        <v>7155</v>
       </c>
       <c r="F973" s="1" t="s">
-        <v>7002</v>
+        <v>7000</v>
       </c>
       <c r="G973" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44576,19 +44594,19 @@
     </row>
     <row r="974" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B974" s="1" t="s">
-        <v>7005</v>
+        <v>7003</v>
       </c>
       <c r="C974" s="1" t="s">
-        <v>7005</v>
+        <v>7003</v>
       </c>
       <c r="D974" s="1" t="s">
-        <v>7006</v>
+        <v>7004</v>
       </c>
       <c r="E974" s="7" t="s">
-        <v>7160</v>
+        <v>7156</v>
       </c>
       <c r="F974" s="1" t="s">
-        <v>7003</v>
+        <v>7001</v>
       </c>
       <c r="G974" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44609,10 +44627,10 @@
         <v>2332</v>
       </c>
       <c r="E975" s="7" t="s">
-        <v>7161</v>
+        <v>7157</v>
       </c>
       <c r="F975" s="1" t="s">
-        <v>7004</v>
+        <v>7002</v>
       </c>
       <c r="G975" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44633,10 +44651,10 @@
         <v>2334</v>
       </c>
       <c r="E976" s="7" t="s">
-        <v>7162</v>
+        <v>7158</v>
       </c>
       <c r="F976" s="1" t="s">
-        <v>7007</v>
+        <v>7005</v>
       </c>
       <c r="G976" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44657,10 +44675,10 @@
         <v>2336</v>
       </c>
       <c r="E977" s="7" t="s">
-        <v>7163</v>
+        <v>7159</v>
       </c>
       <c r="F977" s="1" t="s">
-        <v>7008</v>
+        <v>7006</v>
       </c>
       <c r="G977" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44681,10 +44699,10 @@
         <v>2338</v>
       </c>
       <c r="E978" s="7" t="s">
-        <v>7164</v>
+        <v>7160</v>
       </c>
       <c r="F978" s="1" t="s">
-        <v>7009</v>
+        <v>7007</v>
       </c>
       <c r="G978" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44705,10 +44723,10 @@
         <v>2340</v>
       </c>
       <c r="E979" s="7" t="s">
-        <v>7165</v>
+        <v>7161</v>
       </c>
       <c r="F979" s="1" t="s">
-        <v>7010</v>
+        <v>7008</v>
       </c>
       <c r="G979" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44729,10 +44747,10 @@
         <v>2342</v>
       </c>
       <c r="E980" s="7" t="s">
-        <v>7166</v>
+        <v>7162</v>
       </c>
       <c r="F980" s="1" t="s">
-        <v>7012</v>
+        <v>7010</v>
       </c>
       <c r="G980" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44753,10 +44771,10 @@
         <v>2344</v>
       </c>
       <c r="E981" s="7" t="s">
-        <v>7167</v>
+        <v>7163</v>
       </c>
       <c r="F981" s="1" t="s">
-        <v>7011</v>
+        <v>7009</v>
       </c>
       <c r="G981" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44774,13 +44792,13 @@
         <v>2346</v>
       </c>
       <c r="D982" s="1" t="s">
-        <v>7014</v>
+        <v>7012</v>
       </c>
       <c r="E982" s="7" t="s">
-        <v>7168</v>
+        <v>7164</v>
       </c>
       <c r="F982" s="1" t="s">
-        <v>7013</v>
+        <v>7011</v>
       </c>
       <c r="G982" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44801,10 +44819,10 @@
         <v>2347</v>
       </c>
       <c r="E983" s="7" t="s">
-        <v>7169</v>
+        <v>7165</v>
       </c>
       <c r="F983" s="1" t="s">
-        <v>7015</v>
+        <v>7013</v>
       </c>
       <c r="G983" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44825,10 +44843,10 @@
         <v>2349</v>
       </c>
       <c r="E984" s="7" t="s">
-        <v>7170</v>
+        <v>7166</v>
       </c>
       <c r="F984" s="1" t="s">
-        <v>7016</v>
+        <v>7014</v>
       </c>
       <c r="G984" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44849,10 +44867,10 @@
         <v>2351</v>
       </c>
       <c r="E985" s="7" t="s">
-        <v>7171</v>
+        <v>7167</v>
       </c>
       <c r="F985" s="1" t="s">
-        <v>7017</v>
+        <v>7015</v>
       </c>
       <c r="G985" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44873,10 +44891,10 @@
         <v>2353</v>
       </c>
       <c r="E986" s="7" t="s">
-        <v>7172</v>
+        <v>7168</v>
       </c>
       <c r="F986" s="1" t="s">
-        <v>7018</v>
+        <v>7016</v>
       </c>
       <c r="G986" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44897,10 +44915,10 @@
         <v>2355</v>
       </c>
       <c r="E987" s="7" t="s">
-        <v>7173</v>
+        <v>7169</v>
       </c>
       <c r="F987" s="1" t="s">
-        <v>7019</v>
+        <v>7017</v>
       </c>
       <c r="G987" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44921,10 +44939,10 @@
         <v>2357</v>
       </c>
       <c r="E988" s="7" t="s">
-        <v>7174</v>
+        <v>7170</v>
       </c>
       <c r="F988" s="1" t="s">
-        <v>7020</v>
+        <v>7018</v>
       </c>
       <c r="G988" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44960,10 +44978,10 @@
         <v>2384</v>
       </c>
       <c r="E991" s="7" t="s">
-        <v>7175</v>
+        <v>7171</v>
       </c>
       <c r="F991" s="1" t="s">
-        <v>7021</v>
+        <v>7019</v>
       </c>
       <c r="G991" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44984,10 +45002,10 @@
         <v>2386</v>
       </c>
       <c r="E992" s="7" t="s">
-        <v>7176</v>
+        <v>7172</v>
       </c>
       <c r="F992" s="1" t="s">
-        <v>7022</v>
+        <v>7020</v>
       </c>
       <c r="G992" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45008,10 +45026,10 @@
         <v>2388</v>
       </c>
       <c r="E993" s="7" t="s">
-        <v>7177</v>
+        <v>7173</v>
       </c>
       <c r="F993" s="1" t="s">
-        <v>7023</v>
+        <v>7021</v>
       </c>
       <c r="G993" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45032,10 +45050,10 @@
         <v>2390</v>
       </c>
       <c r="E994" s="7" t="s">
-        <v>7178</v>
+        <v>7174</v>
       </c>
       <c r="F994" s="1" t="s">
-        <v>7024</v>
+        <v>7022</v>
       </c>
       <c r="G994" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45056,10 +45074,10 @@
         <v>2392</v>
       </c>
       <c r="E995" s="7" t="s">
-        <v>7179</v>
+        <v>7175</v>
       </c>
       <c r="F995" s="1" t="s">
-        <v>7025</v>
+        <v>7023</v>
       </c>
       <c r="G995" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45080,10 +45098,10 @@
         <v>2394</v>
       </c>
       <c r="E996" s="7" t="s">
-        <v>7180</v>
+        <v>7176</v>
       </c>
       <c r="F996" s="1" t="s">
-        <v>7026</v>
+        <v>7024</v>
       </c>
       <c r="G996" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45104,10 +45122,10 @@
         <v>2396</v>
       </c>
       <c r="E997" s="7" t="s">
-        <v>7181</v>
+        <v>7177</v>
       </c>
       <c r="F997" s="1" t="s">
-        <v>7027</v>
+        <v>7025</v>
       </c>
       <c r="G997" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45128,10 +45146,10 @@
         <v>2398</v>
       </c>
       <c r="E998" s="7" t="s">
-        <v>7182</v>
+        <v>7178</v>
       </c>
       <c r="F998" s="1" t="s">
-        <v>7028</v>
+        <v>7026</v>
       </c>
       <c r="G998" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45152,10 +45170,10 @@
         <v>1353</v>
       </c>
       <c r="E999" s="7" t="s">
-        <v>7183</v>
+        <v>7179</v>
       </c>
       <c r="F999" s="1" t="s">
-        <v>7029</v>
+        <v>7027</v>
       </c>
       <c r="G999" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45176,10 +45194,10 @@
         <v>2401</v>
       </c>
       <c r="E1000" s="7" t="s">
-        <v>7184</v>
+        <v>7180</v>
       </c>
       <c r="F1000" s="1" t="s">
-        <v>7030</v>
+        <v>7028</v>
       </c>
       <c r="G1000" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45200,10 +45218,10 @@
         <v>2403</v>
       </c>
       <c r="E1001" s="7" t="s">
-        <v>7185</v>
+        <v>7181</v>
       </c>
       <c r="F1001" s="1" t="s">
-        <v>7031</v>
+        <v>7029</v>
       </c>
       <c r="G1001" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45224,10 +45242,10 @@
         <v>2405</v>
       </c>
       <c r="E1002" s="7" t="s">
-        <v>7032</v>
+        <v>7030</v>
       </c>
       <c r="F1002" s="1" t="s">
-        <v>7032</v>
+        <v>7030</v>
       </c>
       <c r="G1002" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45248,10 +45266,10 @@
         <v>2407</v>
       </c>
       <c r="E1003" s="7" t="s">
-        <v>7186</v>
+        <v>7182</v>
       </c>
       <c r="F1003" s="1" t="s">
-        <v>7033</v>
+        <v>7031</v>
       </c>
       <c r="G1003" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45272,10 +45290,10 @@
         <v>2409</v>
       </c>
       <c r="E1004" s="7" t="s">
-        <v>7186</v>
+        <v>7182</v>
       </c>
       <c r="F1004" s="1" t="s">
-        <v>7033</v>
+        <v>7031</v>
       </c>
       <c r="G1004" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45296,10 +45314,10 @@
         <v>2411</v>
       </c>
       <c r="E1005" s="7" t="s">
-        <v>7187</v>
+        <v>7183</v>
       </c>
       <c r="F1005" s="1" t="s">
-        <v>7034</v>
+        <v>7032</v>
       </c>
       <c r="G1005" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45320,10 +45338,10 @@
         <v>2413</v>
       </c>
       <c r="E1006" s="7" t="s">
-        <v>7188</v>
+        <v>7184</v>
       </c>
       <c r="F1006" s="1" t="s">
-        <v>7035</v>
+        <v>7033</v>
       </c>
       <c r="G1006" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45344,10 +45362,10 @@
         <v>2415</v>
       </c>
       <c r="E1007" s="7" t="s">
-        <v>7189</v>
+        <v>7185</v>
       </c>
       <c r="F1007" s="1" t="s">
-        <v>7036</v>
+        <v>7034</v>
       </c>
       <c r="G1007" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45368,10 +45386,10 @@
         <v>2417</v>
       </c>
       <c r="E1008" s="7" t="s">
-        <v>7190</v>
+        <v>7186</v>
       </c>
       <c r="F1008" s="1" t="s">
-        <v>7037</v>
+        <v>7035</v>
       </c>
       <c r="G1008" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45392,10 +45410,10 @@
         <v>2419</v>
       </c>
       <c r="E1009" s="7" t="s">
-        <v>7191</v>
+        <v>7187</v>
       </c>
       <c r="F1009" s="1" t="s">
-        <v>7038</v>
+        <v>7036</v>
       </c>
       <c r="G1009" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45416,10 +45434,10 @@
         <v>2398</v>
       </c>
       <c r="E1010" s="7" t="s">
-        <v>7179</v>
+        <v>7175</v>
       </c>
       <c r="F1010" s="1" t="s">
-        <v>7025</v>
+        <v>7023</v>
       </c>
       <c r="G1010" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45440,10 +45458,10 @@
         <v>2422</v>
       </c>
       <c r="E1011" s="7" t="s">
-        <v>7192</v>
+        <v>7188</v>
       </c>
       <c r="F1011" s="1" t="s">
-        <v>7039</v>
+        <v>7037</v>
       </c>
       <c r="G1011" s="1" t="str">
         <f t="shared" si="18"/>

</xml_diff>

<commit_message>
Speed Master N3 Vocab.xlsx -> Myanmar Definition updated -> Part1 : 29
</commit_message>
<xml_diff>
--- a/preparing/Speed Master N3 Vocab.xlsx
+++ b/preparing/Speed Master N3 Vocab.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7913" uniqueCount="7202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7915" uniqueCount="7203">
   <si>
     <t>yesterday</t>
   </si>
@@ -21023,9 +21023,6 @@
     <t>ဌာန</t>
   </si>
   <si>
-    <t>ပရိ၀ုဏ္၊ နယ္ေျမ</t>
-  </si>
-  <si>
     <t>ေဟာေျပာပို႔ခ်ခ်က္</t>
   </si>
   <si>
@@ -21486,9 +21483,6 @@
   </si>
   <si>
     <t>အထူးပြုခြင်း</t>
-  </si>
-  <si>
-    <t>ပရိဝုဏ်၊ နယ်မြေ</t>
   </si>
   <si>
     <t>ဟောပြောပို့ချချက်</t>
@@ -21632,6 +21626,16 @@
   </si>
   <si>
     <t>Part1 : 28
+Myanmar Definition updated.</t>
+  </si>
+  <si>
+    <t>သင်ကြားမှု ပယ်ဖျက်ခြင်း</t>
+  </si>
+  <si>
+    <t>သင္ၾကားမႈ ပယ္ဖ်က္ျခင္း</t>
+  </si>
+  <si>
+    <t>Part1 : 29
 Myanmar Definition updated.</t>
   </si>
 </sst>
@@ -21671,7 +21675,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -21687,6 +21691,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -21718,7 +21728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -21734,6 +21744,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22041,7 +22053,7 @@
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22216,7 +22228,7 @@
         <v>5404</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>7190</v>
+        <v>7188</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -22230,7 +22242,7 @@
         <v>5404</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>7194</v>
+        <v>7192</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -22244,14 +22256,22 @@
         <v>5404</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>7201</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+        <v>7199</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4">
+        <v>43424</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>5404</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7202</v>
+      </c>
     </row>
     <row r="17" spans="2:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
@@ -22293,8 +22313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1557"/>
   <sheetViews>
-    <sheetView topLeftCell="A930" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C934" sqref="C934"/>
+    <sheetView topLeftCell="A963" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A972" sqref="A972"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" x14ac:dyDescent="0.55000000000000004"/>
@@ -41231,7 +41251,7 @@
         <v>2001</v>
       </c>
       <c r="E829" s="7" t="s">
-        <v>7038</v>
+        <v>7037</v>
       </c>
       <c r="F829" s="1" t="s">
         <v>6860</v>
@@ -41255,7 +41275,7 @@
         <v>2003</v>
       </c>
       <c r="E830" s="7" t="s">
-        <v>7039</v>
+        <v>7038</v>
       </c>
       <c r="F830" s="1" t="s">
         <v>6861</v>
@@ -41279,7 +41299,7 @@
         <v>2005</v>
       </c>
       <c r="E831" s="7" t="s">
-        <v>7040</v>
+        <v>7039</v>
       </c>
       <c r="F831" s="1" t="s">
         <v>6862</v>
@@ -41303,7 +41323,7 @@
         <v>2007</v>
       </c>
       <c r="E832" s="7" t="s">
-        <v>7041</v>
+        <v>7040</v>
       </c>
       <c r="F832" s="1" t="s">
         <v>6863</v>
@@ -41324,7 +41344,7 @@
         <v>6869</v>
       </c>
       <c r="E833" s="7" t="s">
-        <v>7042</v>
+        <v>7041</v>
       </c>
       <c r="F833" s="1" t="s">
         <v>6864</v>
@@ -41348,7 +41368,7 @@
         <v>2009</v>
       </c>
       <c r="E834" s="7" t="s">
-        <v>7043</v>
+        <v>7042</v>
       </c>
       <c r="F834" s="1" t="s">
         <v>6865</v>
@@ -41372,7 +41392,7 @@
         <v>2011</v>
       </c>
       <c r="E835" s="7" t="s">
-        <v>7044</v>
+        <v>7043</v>
       </c>
       <c r="F835" s="1" t="s">
         <v>6866</v>
@@ -41396,7 +41416,7 @@
         <v>2013</v>
       </c>
       <c r="E836" s="7" t="s">
-        <v>7045</v>
+        <v>7044</v>
       </c>
       <c r="F836" s="1" t="s">
         <v>6870</v>
@@ -41420,7 +41440,7 @@
         <v>2015</v>
       </c>
       <c r="E837" s="7" t="s">
-        <v>7046</v>
+        <v>7045</v>
       </c>
       <c r="F837" s="1" t="s">
         <v>6871</v>
@@ -41444,7 +41464,7 @@
         <v>2017</v>
       </c>
       <c r="E838" s="7" t="s">
-        <v>7047</v>
+        <v>7046</v>
       </c>
       <c r="F838" s="1" t="s">
         <v>6872</v>
@@ -41468,7 +41488,7 @@
         <v>2019</v>
       </c>
       <c r="E839" s="7" t="s">
-        <v>7048</v>
+        <v>7047</v>
       </c>
       <c r="F839" s="1" t="s">
         <v>6873</v>
@@ -41492,7 +41512,7 @@
         <v>2021</v>
       </c>
       <c r="E840" s="7" t="s">
-        <v>7049</v>
+        <v>7048</v>
       </c>
       <c r="F840" s="1" t="s">
         <v>6874</v>
@@ -41516,7 +41536,7 @@
         <v>6876</v>
       </c>
       <c r="E841" s="7" t="s">
-        <v>7050</v>
+        <v>7049</v>
       </c>
       <c r="F841" s="1" t="s">
         <v>6875</v>
@@ -41540,7 +41560,7 @@
         <v>2024</v>
       </c>
       <c r="E842" s="7" t="s">
-        <v>7051</v>
+        <v>7050</v>
       </c>
       <c r="F842" s="1" t="s">
         <v>6877</v>
@@ -41564,7 +41584,7 @@
         <v>2025</v>
       </c>
       <c r="E843" s="7" t="s">
-        <v>7052</v>
+        <v>7051</v>
       </c>
       <c r="F843" s="1" t="s">
         <v>6878</v>
@@ -41588,7 +41608,7 @@
         <v>6880</v>
       </c>
       <c r="E844" s="7" t="s">
-        <v>7053</v>
+        <v>7052</v>
       </c>
       <c r="F844" s="1" t="s">
         <v>6879</v>
@@ -41612,7 +41632,7 @@
         <v>2028</v>
       </c>
       <c r="E845" s="7" t="s">
-        <v>7054</v>
+        <v>7053</v>
       </c>
       <c r="F845" s="1" t="s">
         <v>6881</v>
@@ -41636,7 +41656,7 @@
         <v>2030</v>
       </c>
       <c r="E846" s="7" t="s">
-        <v>7055</v>
+        <v>7054</v>
       </c>
       <c r="F846" s="1" t="s">
         <v>6882</v>
@@ -41684,7 +41704,7 @@
         <v>2034</v>
       </c>
       <c r="E848" s="7" t="s">
-        <v>7056</v>
+        <v>7055</v>
       </c>
       <c r="F848" s="1" t="s">
         <v>6884</v>
@@ -41708,7 +41728,7 @@
         <v>2036</v>
       </c>
       <c r="E849" s="7" t="s">
-        <v>7057</v>
+        <v>7056</v>
       </c>
       <c r="F849" s="1" t="s">
         <v>6885</v>
@@ -41732,7 +41752,7 @@
         <v>2038</v>
       </c>
       <c r="E850" s="7" t="s">
-        <v>7058</v>
+        <v>7057</v>
       </c>
       <c r="F850" s="1" t="s">
         <v>6886</v>
@@ -41756,7 +41776,7 @@
         <v>2040</v>
       </c>
       <c r="E851" s="7" t="s">
-        <v>7059</v>
+        <v>7058</v>
       </c>
       <c r="F851" s="1" t="s">
         <v>6887</v>
@@ -41780,7 +41800,7 @@
         <v>6890</v>
       </c>
       <c r="E852" s="7" t="s">
-        <v>7060</v>
+        <v>7059</v>
       </c>
       <c r="F852" s="1" t="s">
         <v>6888</v>
@@ -41804,7 +41824,7 @@
         <v>2043</v>
       </c>
       <c r="E853" s="7" t="s">
-        <v>7060</v>
+        <v>7059</v>
       </c>
       <c r="F853" s="1" t="s">
         <v>6888</v>
@@ -41828,7 +41848,7 @@
         <v>2045</v>
       </c>
       <c r="E854" s="7" t="s">
-        <v>7061</v>
+        <v>7060</v>
       </c>
       <c r="F854" s="1" t="s">
         <v>6889</v>
@@ -41876,7 +41896,7 @@
         <v>2049</v>
       </c>
       <c r="E856" s="7" t="s">
-        <v>7062</v>
+        <v>7061</v>
       </c>
       <c r="F856" s="1" t="s">
         <v>6891</v>
@@ -41900,7 +41920,7 @@
         <v>2051</v>
       </c>
       <c r="E857" s="7" t="s">
-        <v>7063</v>
+        <v>7062</v>
       </c>
       <c r="F857" s="1" t="s">
         <v>6892</v>
@@ -41924,7 +41944,7 @@
         <v>2053</v>
       </c>
       <c r="E858" s="7" t="s">
-        <v>7064</v>
+        <v>7063</v>
       </c>
       <c r="F858" s="1" t="s">
         <v>6893</v>
@@ -41948,7 +41968,7 @@
         <v>2055</v>
       </c>
       <c r="E859" s="7" t="s">
-        <v>7065</v>
+        <v>7064</v>
       </c>
       <c r="F859" s="1" t="s">
         <v>6894</v>
@@ -41972,7 +41992,7 @@
         <v>2057</v>
       </c>
       <c r="E860" s="7" t="s">
-        <v>7066</v>
+        <v>7065</v>
       </c>
       <c r="F860" s="1" t="s">
         <v>6895</v>
@@ -41996,7 +42016,7 @@
         <v>2059</v>
       </c>
       <c r="E861" s="7" t="s">
-        <v>7067</v>
+        <v>7066</v>
       </c>
       <c r="F861" s="1" t="s">
         <v>6896</v>
@@ -42020,7 +42040,7 @@
         <v>2061</v>
       </c>
       <c r="E862" s="7" t="s">
-        <v>7068</v>
+        <v>7067</v>
       </c>
       <c r="F862" s="1" t="s">
         <v>6897</v>
@@ -42044,7 +42064,7 @@
         <v>2063</v>
       </c>
       <c r="E863" s="7" t="s">
-        <v>7069</v>
+        <v>7068</v>
       </c>
       <c r="F863" s="1" t="s">
         <v>6898</v>
@@ -42068,7 +42088,7 @@
         <v>6899</v>
       </c>
       <c r="E864" s="7" t="s">
-        <v>7069</v>
+        <v>7068</v>
       </c>
       <c r="F864" s="1" t="s">
         <v>6898</v>
@@ -42092,7 +42112,7 @@
         <v>2066</v>
       </c>
       <c r="E865" s="7" t="s">
-        <v>7070</v>
+        <v>7069</v>
       </c>
       <c r="F865" s="1" t="s">
         <v>6900</v>
@@ -42116,7 +42136,7 @@
         <v>2068</v>
       </c>
       <c r="E866" s="7" t="s">
-        <v>7071</v>
+        <v>7070</v>
       </c>
       <c r="F866" s="1" t="s">
         <v>6901</v>
@@ -42140,7 +42160,7 @@
         <v>2070</v>
       </c>
       <c r="E867" s="7" t="s">
-        <v>7072</v>
+        <v>7071</v>
       </c>
       <c r="F867" s="1" t="s">
         <v>6902</v>
@@ -42164,7 +42184,7 @@
         <v>2072</v>
       </c>
       <c r="E868" s="7" t="s">
-        <v>7073</v>
+        <v>7072</v>
       </c>
       <c r="F868" s="1" t="s">
         <v>6903</v>
@@ -42188,7 +42208,7 @@
         <v>2074</v>
       </c>
       <c r="E869" s="7" t="s">
-        <v>7074</v>
+        <v>7073</v>
       </c>
       <c r="F869" s="1" t="s">
         <v>6904</v>
@@ -42212,7 +42232,7 @@
         <v>2076</v>
       </c>
       <c r="E870" s="7" t="s">
-        <v>7075</v>
+        <v>7074</v>
       </c>
       <c r="F870" s="1" t="s">
         <v>6905</v>
@@ -42236,7 +42256,7 @@
         <v>2078</v>
       </c>
       <c r="E871" s="7" t="s">
-        <v>7076</v>
+        <v>7075</v>
       </c>
       <c r="F871" s="1" t="s">
         <v>6906</v>
@@ -42260,7 +42280,7 @@
         <v>2080</v>
       </c>
       <c r="E872" s="7" t="s">
-        <v>7077</v>
+        <v>7076</v>
       </c>
       <c r="F872" s="1" t="s">
         <v>6907</v>
@@ -42284,7 +42304,7 @@
         <v>2082</v>
       </c>
       <c r="E873" s="7" t="s">
-        <v>7078</v>
+        <v>7077</v>
       </c>
       <c r="F873" s="1" t="s">
         <v>6908</v>
@@ -42323,16 +42343,16 @@
         <v>815</v>
       </c>
       <c r="B875" s="1" t="s">
+        <v>7189</v>
+      </c>
+      <c r="C875" s="1" t="s">
+        <v>7190</v>
+      </c>
+      <c r="D875" s="1" t="s">
         <v>7191</v>
       </c>
-      <c r="C875" s="1" t="s">
-        <v>7192</v>
-      </c>
-      <c r="D875" s="1" t="s">
-        <v>7193</v>
-      </c>
       <c r="E875" s="7" t="s">
-        <v>7079</v>
+        <v>7078</v>
       </c>
       <c r="F875" s="1" t="s">
         <v>6910</v>
@@ -42356,7 +42376,7 @@
         <v>2086</v>
       </c>
       <c r="E876" s="7" t="s">
-        <v>7080</v>
+        <v>7079</v>
       </c>
       <c r="F876" s="1" t="s">
         <v>6911</v>
@@ -42380,7 +42400,7 @@
         <v>2089</v>
       </c>
       <c r="E877" s="7" t="s">
-        <v>7081</v>
+        <v>7080</v>
       </c>
       <c r="F877" s="1" t="s">
         <v>6912</v>
@@ -42404,7 +42424,7 @@
         <v>6913</v>
       </c>
       <c r="E878" s="7" t="s">
-        <v>7082</v>
+        <v>7081</v>
       </c>
       <c r="F878" s="1" t="s">
         <v>6914</v>
@@ -42428,7 +42448,7 @@
         <v>2093</v>
       </c>
       <c r="E879" s="7" t="s">
-        <v>7083</v>
+        <v>7082</v>
       </c>
       <c r="F879" s="1" t="s">
         <v>6915</v>
@@ -42452,7 +42472,7 @@
         <v>2088</v>
       </c>
       <c r="E880" s="1" t="s">
-        <v>7084</v>
+        <v>7083</v>
       </c>
       <c r="F880" s="1" t="s">
         <v>6916</v>
@@ -42473,7 +42493,7 @@
         <v>2095</v>
       </c>
       <c r="E881" s="7" t="s">
-        <v>7085</v>
+        <v>7084</v>
       </c>
       <c r="F881" s="1" t="s">
         <v>6918</v>
@@ -42497,7 +42517,7 @@
         <v>2097</v>
       </c>
       <c r="E882" s="7" t="s">
-        <v>7086</v>
+        <v>7085</v>
       </c>
       <c r="F882" s="1" t="s">
         <v>6917</v>
@@ -42521,7 +42541,7 @@
         <v>2099</v>
       </c>
       <c r="E883" s="7" t="s">
-        <v>7087</v>
+        <v>7086</v>
       </c>
       <c r="F883" s="1" t="s">
         <v>6919</v>
@@ -42545,7 +42565,7 @@
         <v>2101</v>
       </c>
       <c r="E884" s="7" t="s">
-        <v>7088</v>
+        <v>7087</v>
       </c>
       <c r="F884" s="1" t="s">
         <v>6920</v>
@@ -42569,7 +42589,7 @@
         <v>2103</v>
       </c>
       <c r="E885" s="7" t="s">
-        <v>7089</v>
+        <v>7088</v>
       </c>
       <c r="F885" s="1" t="s">
         <v>6921</v>
@@ -42593,7 +42613,7 @@
         <v>2105</v>
       </c>
       <c r="E886" s="7" t="s">
-        <v>7090</v>
+        <v>7089</v>
       </c>
       <c r="F886" s="1" t="s">
         <v>6922</v>
@@ -42617,7 +42637,7 @@
         <v>2107</v>
       </c>
       <c r="E887" s="7" t="s">
-        <v>7091</v>
+        <v>7090</v>
       </c>
       <c r="F887" s="1" t="s">
         <v>6923</v>
@@ -42641,7 +42661,7 @@
         <v>2109</v>
       </c>
       <c r="E888" s="7" t="s">
-        <v>7092</v>
+        <v>7091</v>
       </c>
       <c r="F888" s="1" t="s">
         <v>6924</v>
@@ -42665,7 +42685,7 @@
         <v>6004</v>
       </c>
       <c r="E889" s="7" t="s">
-        <v>7093</v>
+        <v>7092</v>
       </c>
       <c r="F889" s="1" t="s">
         <v>6925</v>
@@ -42689,7 +42709,7 @@
         <v>1954</v>
       </c>
       <c r="E890" s="7" t="s">
-        <v>7094</v>
+        <v>7093</v>
       </c>
       <c r="F890" s="1" t="s">
         <v>6926</v>
@@ -42713,7 +42733,7 @@
         <v>6927</v>
       </c>
       <c r="E891" s="7" t="s">
-        <v>7095</v>
+        <v>7094</v>
       </c>
       <c r="F891" s="1" t="s">
         <v>6928</v>
@@ -42737,7 +42757,7 @@
         <v>2112</v>
       </c>
       <c r="E892" s="7" t="s">
-        <v>7096</v>
+        <v>7095</v>
       </c>
       <c r="F892" s="1" t="s">
         <v>6929</v>
@@ -42761,7 +42781,7 @@
         <v>2114</v>
       </c>
       <c r="E893" s="7" t="s">
-        <v>7097</v>
+        <v>7096</v>
       </c>
       <c r="F893" s="1" t="s">
         <v>6930</v>
@@ -42785,7 +42805,7 @@
         <v>2116</v>
       </c>
       <c r="E894" s="7" t="s">
-        <v>7098</v>
+        <v>7097</v>
       </c>
       <c r="F894" s="1" t="s">
         <v>6931</v>
@@ -42809,7 +42829,7 @@
         <v>2118</v>
       </c>
       <c r="E895" s="7" t="s">
-        <v>7099</v>
+        <v>7098</v>
       </c>
       <c r="F895" s="1" t="s">
         <v>6932</v>
@@ -42833,7 +42853,7 @@
         <v>2120</v>
       </c>
       <c r="E896" s="7" t="s">
-        <v>7100</v>
+        <v>7099</v>
       </c>
       <c r="F896" s="1" t="s">
         <v>6933</v>
@@ -42857,7 +42877,7 @@
         <v>2122</v>
       </c>
       <c r="E897" s="7" t="s">
-        <v>7101</v>
+        <v>7100</v>
       </c>
       <c r="F897" s="1" t="s">
         <v>6934</v>
@@ -42896,7 +42916,7 @@
         <v>2155</v>
       </c>
       <c r="E900" s="7" t="s">
-        <v>7102</v>
+        <v>7101</v>
       </c>
       <c r="F900" s="1" t="s">
         <v>6935</v>
@@ -42920,7 +42940,7 @@
         <v>2157</v>
       </c>
       <c r="E901" s="7" t="s">
-        <v>7102</v>
+        <v>7101</v>
       </c>
       <c r="F901" s="1" t="s">
         <v>6935</v>
@@ -42968,7 +42988,7 @@
         <v>2161</v>
       </c>
       <c r="E903" s="7" t="s">
-        <v>7103</v>
+        <v>7102</v>
       </c>
       <c r="F903" s="1" t="s">
         <v>6936</v>
@@ -43016,7 +43036,7 @@
         <v>2164</v>
       </c>
       <c r="E905" s="7" t="s">
-        <v>7104</v>
+        <v>7103</v>
       </c>
       <c r="F905" s="1" t="s">
         <v>6937</v>
@@ -43040,7 +43060,7 @@
         <v>2166</v>
       </c>
       <c r="E906" s="7" t="s">
-        <v>7105</v>
+        <v>7104</v>
       </c>
       <c r="F906" s="1" t="s">
         <v>6938</v>
@@ -43064,7 +43084,7 @@
         <v>2168</v>
       </c>
       <c r="E907" s="7" t="s">
-        <v>7106</v>
+        <v>7105</v>
       </c>
       <c r="F907" s="1" t="s">
         <v>6939</v>
@@ -43088,7 +43108,7 @@
         <v>2170</v>
       </c>
       <c r="E908" s="7" t="s">
-        <v>7107</v>
+        <v>7106</v>
       </c>
       <c r="F908" s="1" t="s">
         <v>6940</v>
@@ -43112,7 +43132,7 @@
         <v>2172</v>
       </c>
       <c r="E909" s="7" t="s">
-        <v>7108</v>
+        <v>7107</v>
       </c>
       <c r="F909" s="1" t="s">
         <v>6941</v>
@@ -43160,7 +43180,7 @@
         <v>2176</v>
       </c>
       <c r="E911" s="7" t="s">
-        <v>7109</v>
+        <v>7108</v>
       </c>
       <c r="F911" s="1" t="s">
         <v>6942</v>
@@ -43208,7 +43228,7 @@
         <v>2180</v>
       </c>
       <c r="E913" s="7" t="s">
-        <v>7110</v>
+        <v>7109</v>
       </c>
       <c r="F913" s="1" t="s">
         <v>6943</v>
@@ -43232,7 +43252,7 @@
         <v>2182</v>
       </c>
       <c r="E914" s="7" t="s">
-        <v>7111</v>
+        <v>7110</v>
       </c>
       <c r="F914" s="1" t="s">
         <v>6944</v>
@@ -43256,7 +43276,7 @@
         <v>2184</v>
       </c>
       <c r="E915" s="7" t="s">
-        <v>7112</v>
+        <v>7111</v>
       </c>
       <c r="F915" s="1" t="s">
         <v>6945</v>
@@ -43280,7 +43300,7 @@
         <v>2186</v>
       </c>
       <c r="E916" s="7" t="s">
-        <v>7113</v>
+        <v>7112</v>
       </c>
       <c r="F916" s="1" t="s">
         <v>6946</v>
@@ -43304,7 +43324,7 @@
         <v>2187</v>
       </c>
       <c r="E917" s="7" t="s">
-        <v>7114</v>
+        <v>7113</v>
       </c>
       <c r="F917" s="1" t="s">
         <v>6947</v>
@@ -43328,7 +43348,7 @@
         <v>2189</v>
       </c>
       <c r="E918" s="7" t="s">
-        <v>7115</v>
+        <v>7114</v>
       </c>
       <c r="F918" s="1" t="s">
         <v>6948</v>
@@ -43352,7 +43372,7 @@
         <v>2191</v>
       </c>
       <c r="E919" s="7" t="s">
-        <v>7116</v>
+        <v>7115</v>
       </c>
       <c r="F919" s="1" t="s">
         <v>6949</v>
@@ -43400,7 +43420,7 @@
         <v>2195</v>
       </c>
       <c r="E921" s="7" t="s">
-        <v>7117</v>
+        <v>7116</v>
       </c>
       <c r="F921" s="1" t="s">
         <v>6951</v>
@@ -43448,7 +43468,7 @@
         <v>2199</v>
       </c>
       <c r="E923" s="7" t="s">
-        <v>7118</v>
+        <v>7117</v>
       </c>
       <c r="F923" s="1" t="s">
         <v>6953</v>
@@ -43472,7 +43492,7 @@
         <v>2201</v>
       </c>
       <c r="E924" s="7" t="s">
-        <v>7119</v>
+        <v>7118</v>
       </c>
       <c r="F924" s="1" t="s">
         <v>6954</v>
@@ -43496,7 +43516,7 @@
         <v>2203</v>
       </c>
       <c r="E925" s="7" t="s">
-        <v>7120</v>
+        <v>7119</v>
       </c>
       <c r="F925" s="1" t="s">
         <v>6955</v>
@@ -43520,7 +43540,7 @@
         <v>2205</v>
       </c>
       <c r="E926" s="7" t="s">
-        <v>7121</v>
+        <v>7120</v>
       </c>
       <c r="F926" s="1" t="s">
         <v>6956</v>
@@ -43568,7 +43588,7 @@
         <v>2209</v>
       </c>
       <c r="E928" s="7" t="s">
-        <v>7122</v>
+        <v>7121</v>
       </c>
       <c r="F928" s="1" t="s">
         <v>6958</v>
@@ -43592,7 +43612,7 @@
         <v>2211</v>
       </c>
       <c r="E929" s="7" t="s">
-        <v>7123</v>
+        <v>7122</v>
       </c>
       <c r="F929" s="1" t="s">
         <v>6959</v>
@@ -43616,7 +43636,7 @@
         <v>6961</v>
       </c>
       <c r="E930" s="7" t="s">
-        <v>7124</v>
+        <v>7123</v>
       </c>
       <c r="F930" s="1" t="s">
         <v>6960</v>
@@ -43655,7 +43675,7 @@
         <v>6964</v>
       </c>
       <c r="E933" s="7" t="s">
-        <v>7125</v>
+        <v>7124</v>
       </c>
       <c r="F933" s="1" t="s">
         <v>6962</v>
@@ -43679,7 +43699,7 @@
         <v>2239</v>
       </c>
       <c r="E934" s="7" t="s">
-        <v>7126</v>
+        <v>7125</v>
       </c>
       <c r="F934" s="1" t="s">
         <v>6963</v>
@@ -43703,10 +43723,10 @@
         <v>2241</v>
       </c>
       <c r="E935" s="7" t="s">
-        <v>7195</v>
+        <v>7193</v>
       </c>
       <c r="F935" s="1" t="s">
-        <v>7196</v>
+        <v>7194</v>
       </c>
       <c r="G935" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43727,7 +43747,7 @@
         <v>6966</v>
       </c>
       <c r="E936" s="7" t="s">
-        <v>7127</v>
+        <v>7126</v>
       </c>
       <c r="F936" s="1" t="s">
         <v>6965</v>
@@ -43751,10 +43771,10 @@
         <v>2245</v>
       </c>
       <c r="E937" s="7" t="s">
-        <v>7197</v>
+        <v>7195</v>
       </c>
       <c r="F937" s="1" t="s">
-        <v>7198</v>
+        <v>7196</v>
       </c>
       <c r="G937" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43766,7 +43786,7 @@
         <v>873</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>7189</v>
+        <v>7187</v>
       </c>
       <c r="C938" s="1" t="s">
         <v>2248</v>
@@ -43775,10 +43795,10 @@
         <v>2247</v>
       </c>
       <c r="E938" s="7" t="s">
-        <v>7199</v>
+        <v>7197</v>
       </c>
       <c r="F938" s="1" t="s">
-        <v>7200</v>
+        <v>7198</v>
       </c>
       <c r="G938" s="1" t="str">
         <f t="shared" si="17"/>
@@ -43823,7 +43843,7 @@
         <v>6969</v>
       </c>
       <c r="E940" s="7" t="s">
-        <v>7128</v>
+        <v>7127</v>
       </c>
       <c r="F940" s="1" t="s">
         <v>6968</v>
@@ -43847,7 +43867,7 @@
         <v>2252</v>
       </c>
       <c r="E941" s="7" t="s">
-        <v>7129</v>
+        <v>7128</v>
       </c>
       <c r="F941" s="1" t="s">
         <v>6970</v>
@@ -43871,7 +43891,7 @@
         <v>2254</v>
       </c>
       <c r="E942" s="7" t="s">
-        <v>7130</v>
+        <v>7129</v>
       </c>
       <c r="F942" s="1" t="s">
         <v>6971</v>
@@ -43895,7 +43915,7 @@
         <v>1011</v>
       </c>
       <c r="E943" s="7" t="s">
-        <v>7131</v>
+        <v>7130</v>
       </c>
       <c r="F943" s="1" t="s">
         <v>6972</v>
@@ -43919,7 +43939,7 @@
         <v>2257</v>
       </c>
       <c r="E944" s="7" t="s">
-        <v>7132</v>
+        <v>7131</v>
       </c>
       <c r="F944" s="1" t="s">
         <v>6973</v>
@@ -43943,7 +43963,7 @@
         <v>2259</v>
       </c>
       <c r="E945" s="7" t="s">
-        <v>7133</v>
+        <v>7132</v>
       </c>
       <c r="F945" s="1" t="s">
         <v>6974</v>
@@ -43967,7 +43987,7 @@
         <v>2261</v>
       </c>
       <c r="E946" s="7" t="s">
-        <v>7134</v>
+        <v>7133</v>
       </c>
       <c r="F946" s="1" t="s">
         <v>6975</v>
@@ -43991,7 +44011,7 @@
         <v>2263</v>
       </c>
       <c r="E947" s="7" t="s">
-        <v>7135</v>
+        <v>7134</v>
       </c>
       <c r="F947" s="1" t="s">
         <v>6976</v>
@@ -44015,7 +44035,7 @@
         <v>2265</v>
       </c>
       <c r="E948" s="7" t="s">
-        <v>7136</v>
+        <v>7135</v>
       </c>
       <c r="F948" s="1" t="s">
         <v>6977</v>
@@ -44039,7 +44059,7 @@
         <v>2267</v>
       </c>
       <c r="E949" s="7" t="s">
-        <v>7137</v>
+        <v>7136</v>
       </c>
       <c r="F949" s="1" t="s">
         <v>6978</v>
@@ -44063,7 +44083,7 @@
         <v>2269</v>
       </c>
       <c r="E950" s="7" t="s">
-        <v>7138</v>
+        <v>7137</v>
       </c>
       <c r="F950" s="1" t="s">
         <v>6979</v>
@@ -44087,7 +44107,7 @@
         <v>2271</v>
       </c>
       <c r="E951" s="7" t="s">
-        <v>7139</v>
+        <v>7138</v>
       </c>
       <c r="F951" s="1" t="s">
         <v>6980</v>
@@ -44111,7 +44131,7 @@
         <v>2273</v>
       </c>
       <c r="E952" s="7" t="s">
-        <v>7140</v>
+        <v>7139</v>
       </c>
       <c r="F952" s="1" t="s">
         <v>6981</v>
@@ -44159,7 +44179,7 @@
         <v>6984</v>
       </c>
       <c r="E954" s="7" t="s">
-        <v>7141</v>
+        <v>7140</v>
       </c>
       <c r="F954" s="1" t="s">
         <v>6985</v>
@@ -44183,7 +44203,7 @@
         <v>2277</v>
       </c>
       <c r="E955" s="7" t="s">
-        <v>7142</v>
+        <v>7141</v>
       </c>
       <c r="F955" s="1" t="s">
         <v>6986</v>
@@ -44207,7 +44227,7 @@
         <v>2279</v>
       </c>
       <c r="E956" s="7" t="s">
-        <v>7143</v>
+        <v>7142</v>
       </c>
       <c r="F956" s="1" t="s">
         <v>6987</v>
@@ -44231,7 +44251,7 @@
         <v>2281</v>
       </c>
       <c r="E957" s="7" t="s">
-        <v>7131</v>
+        <v>7130</v>
       </c>
       <c r="F957" s="1" t="s">
         <v>6972</v>
@@ -44255,7 +44275,7 @@
         <v>2283</v>
       </c>
       <c r="E958" s="7" t="s">
-        <v>7144</v>
+        <v>7143</v>
       </c>
       <c r="F958" s="1" t="s">
         <v>6988</v>
@@ -44279,7 +44299,7 @@
         <v>2285</v>
       </c>
       <c r="E959" s="7" t="s">
-        <v>7145</v>
+        <v>7144</v>
       </c>
       <c r="F959" s="1" t="s">
         <v>6989</v>
@@ -44318,7 +44338,7 @@
         <v>2310</v>
       </c>
       <c r="E962" s="7" t="s">
-        <v>7146</v>
+        <v>7145</v>
       </c>
       <c r="F962" s="1" t="s">
         <v>6990</v>
@@ -44342,7 +44362,7 @@
         <v>2312</v>
       </c>
       <c r="E963" s="7" t="s">
-        <v>7147</v>
+        <v>7146</v>
       </c>
       <c r="F963" s="1" t="s">
         <v>6991</v>
@@ -44366,7 +44386,7 @@
         <v>2314</v>
       </c>
       <c r="E964" s="7" t="s">
-        <v>7148</v>
+        <v>7147</v>
       </c>
       <c r="F964" s="1" t="s">
         <v>6992</v>
@@ -44390,7 +44410,7 @@
         <v>2316</v>
       </c>
       <c r="E965" s="7" t="s">
-        <v>7149</v>
+        <v>7148</v>
       </c>
       <c r="F965" s="1" t="s">
         <v>6993</v>
@@ -44414,7 +44434,7 @@
         <v>2318</v>
       </c>
       <c r="E966" s="7" t="s">
-        <v>7150</v>
+        <v>7149</v>
       </c>
       <c r="F966" s="1" t="s">
         <v>6994</v>
@@ -44438,7 +44458,7 @@
         <v>2320</v>
       </c>
       <c r="E967" s="7" t="s">
-        <v>7151</v>
+        <v>7150</v>
       </c>
       <c r="F967" s="1" t="s">
         <v>6995</v>
@@ -44462,7 +44482,7 @@
         <v>2322</v>
       </c>
       <c r="E968" s="7" t="s">
-        <v>7152</v>
+        <v>7151</v>
       </c>
       <c r="F968" s="1" t="s">
         <v>6996</v>
@@ -44486,7 +44506,7 @@
         <v>2324</v>
       </c>
       <c r="E969" s="7" t="s">
-        <v>7153</v>
+        <v>7152</v>
       </c>
       <c r="F969" s="1" t="s">
         <v>6997</v>
@@ -44534,7 +44554,7 @@
         <v>2281</v>
       </c>
       <c r="E971" s="10" t="s">
-        <v>7131</v>
+        <v>7130</v>
       </c>
       <c r="F971" s="8" t="s">
         <v>6972</v>
@@ -44557,56 +44577,56 @@
       <c r="D972" s="1" t="s">
         <v>2328</v>
       </c>
-      <c r="E972" s="7" t="s">
-        <v>7154</v>
-      </c>
-      <c r="F972" s="1" t="s">
+      <c r="E972" s="12" t="s">
+        <v>7153</v>
+      </c>
+      <c r="F972" s="11" t="s">
         <v>6999</v>
       </c>
       <c r="G972" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>lecture ; ပရိဝုဏ်၊ နယ်မြေ ; ပရိ၀ုဏ္၊ နယ္ေျမ</v>
-      </c>
-    </row>
-    <row r="973" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A973" s="1">
+        <f>CONCATENATE(D972, " ; ",E972," ; ",F972)</f>
+        <v>lecture ; ဟောပြောပို့ချချက် ; ေဟာေျပာပို႔ခ်ခ်က္</v>
+      </c>
+    </row>
+    <row r="973" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A973" s="11">
         <v>906</v>
       </c>
-      <c r="B973" s="1" t="s">
+      <c r="B973" s="11" t="s">
         <v>2369</v>
       </c>
-      <c r="C973" s="1" t="s">
+      <c r="C973" s="11" t="s">
         <v>2331</v>
       </c>
-      <c r="D973" s="1" t="s">
+      <c r="D973" s="11" t="s">
         <v>2330</v>
       </c>
-      <c r="E973" s="7" t="s">
-        <v>7155</v>
-      </c>
-      <c r="F973" s="1" t="s">
-        <v>7000</v>
+      <c r="E973" s="11" t="s">
+        <v>7200</v>
+      </c>
+      <c r="F973" s="11" t="s">
+        <v>7201</v>
       </c>
       <c r="G973" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>lecture cancellation ; ဟောပြောပို့ချချက် ; ေဟာေျပာပို႔ခ်ခ်က္</v>
+        <f>CONCATENATE(D973, " ; ",E973," ; ",F973)</f>
+        <v>lecture cancellation ; သင်ကြားမှု ပယ်ဖျက်ခြင်း ; သင္ၾကားမႈ ပယ္ဖ်က္ျခင္း</v>
       </c>
     </row>
     <row r="974" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B974" s="1" t="s">
+        <v>7002</v>
+      </c>
+      <c r="C974" s="1" t="s">
+        <v>7002</v>
+      </c>
+      <c r="D974" s="1" t="s">
         <v>7003</v>
       </c>
-      <c r="C974" s="1" t="s">
-        <v>7003</v>
-      </c>
-      <c r="D974" s="1" t="s">
-        <v>7004</v>
-      </c>
       <c r="E974" s="7" t="s">
-        <v>7156</v>
+        <v>7154</v>
       </c>
       <c r="F974" s="1" t="s">
-        <v>7001</v>
+        <v>7000</v>
       </c>
       <c r="G974" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44627,10 +44647,10 @@
         <v>2332</v>
       </c>
       <c r="E975" s="7" t="s">
-        <v>7157</v>
+        <v>7155</v>
       </c>
       <c r="F975" s="1" t="s">
-        <v>7002</v>
+        <v>7001</v>
       </c>
       <c r="G975" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44651,10 +44671,10 @@
         <v>2334</v>
       </c>
       <c r="E976" s="7" t="s">
-        <v>7158</v>
+        <v>7156</v>
       </c>
       <c r="F976" s="1" t="s">
-        <v>7005</v>
+        <v>7004</v>
       </c>
       <c r="G976" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44675,10 +44695,10 @@
         <v>2336</v>
       </c>
       <c r="E977" s="7" t="s">
-        <v>7159</v>
+        <v>7157</v>
       </c>
       <c r="F977" s="1" t="s">
-        <v>7006</v>
+        <v>7005</v>
       </c>
       <c r="G977" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44699,10 +44719,10 @@
         <v>2338</v>
       </c>
       <c r="E978" s="7" t="s">
-        <v>7160</v>
+        <v>7158</v>
       </c>
       <c r="F978" s="1" t="s">
-        <v>7007</v>
+        <v>7006</v>
       </c>
       <c r="G978" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44723,10 +44743,10 @@
         <v>2340</v>
       </c>
       <c r="E979" s="7" t="s">
-        <v>7161</v>
+        <v>7159</v>
       </c>
       <c r="F979" s="1" t="s">
-        <v>7008</v>
+        <v>7007</v>
       </c>
       <c r="G979" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44747,10 +44767,10 @@
         <v>2342</v>
       </c>
       <c r="E980" s="7" t="s">
-        <v>7162</v>
+        <v>7160</v>
       </c>
       <c r="F980" s="1" t="s">
-        <v>7010</v>
+        <v>7009</v>
       </c>
       <c r="G980" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44771,10 +44791,10 @@
         <v>2344</v>
       </c>
       <c r="E981" s="7" t="s">
-        <v>7163</v>
+        <v>7161</v>
       </c>
       <c r="F981" s="1" t="s">
-        <v>7009</v>
+        <v>7008</v>
       </c>
       <c r="G981" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44792,13 +44812,13 @@
         <v>2346</v>
       </c>
       <c r="D982" s="1" t="s">
-        <v>7012</v>
+        <v>7011</v>
       </c>
       <c r="E982" s="7" t="s">
-        <v>7164</v>
+        <v>7162</v>
       </c>
       <c r="F982" s="1" t="s">
-        <v>7011</v>
+        <v>7010</v>
       </c>
       <c r="G982" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44819,10 +44839,10 @@
         <v>2347</v>
       </c>
       <c r="E983" s="7" t="s">
-        <v>7165</v>
+        <v>7163</v>
       </c>
       <c r="F983" s="1" t="s">
-        <v>7013</v>
+        <v>7012</v>
       </c>
       <c r="G983" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44843,10 +44863,10 @@
         <v>2349</v>
       </c>
       <c r="E984" s="7" t="s">
-        <v>7166</v>
+        <v>7164</v>
       </c>
       <c r="F984" s="1" t="s">
-        <v>7014</v>
+        <v>7013</v>
       </c>
       <c r="G984" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44867,10 +44887,10 @@
         <v>2351</v>
       </c>
       <c r="E985" s="7" t="s">
-        <v>7167</v>
+        <v>7165</v>
       </c>
       <c r="F985" s="1" t="s">
-        <v>7015</v>
+        <v>7014</v>
       </c>
       <c r="G985" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44891,10 +44911,10 @@
         <v>2353</v>
       </c>
       <c r="E986" s="7" t="s">
-        <v>7168</v>
+        <v>7166</v>
       </c>
       <c r="F986" s="1" t="s">
-        <v>7016</v>
+        <v>7015</v>
       </c>
       <c r="G986" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44915,10 +44935,10 @@
         <v>2355</v>
       </c>
       <c r="E987" s="7" t="s">
-        <v>7169</v>
+        <v>7167</v>
       </c>
       <c r="F987" s="1" t="s">
-        <v>7017</v>
+        <v>7016</v>
       </c>
       <c r="G987" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44939,10 +44959,10 @@
         <v>2357</v>
       </c>
       <c r="E988" s="7" t="s">
-        <v>7170</v>
+        <v>7168</v>
       </c>
       <c r="F988" s="1" t="s">
-        <v>7018</v>
+        <v>7017</v>
       </c>
       <c r="G988" s="1" t="str">
         <f t="shared" si="18"/>
@@ -44978,10 +44998,10 @@
         <v>2384</v>
       </c>
       <c r="E991" s="7" t="s">
-        <v>7171</v>
+        <v>7169</v>
       </c>
       <c r="F991" s="1" t="s">
-        <v>7019</v>
+        <v>7018</v>
       </c>
       <c r="G991" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45002,10 +45022,10 @@
         <v>2386</v>
       </c>
       <c r="E992" s="7" t="s">
-        <v>7172</v>
+        <v>7170</v>
       </c>
       <c r="F992" s="1" t="s">
-        <v>7020</v>
+        <v>7019</v>
       </c>
       <c r="G992" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45026,10 +45046,10 @@
         <v>2388</v>
       </c>
       <c r="E993" s="7" t="s">
-        <v>7173</v>
+        <v>7171</v>
       </c>
       <c r="F993" s="1" t="s">
-        <v>7021</v>
+        <v>7020</v>
       </c>
       <c r="G993" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45050,10 +45070,10 @@
         <v>2390</v>
       </c>
       <c r="E994" s="7" t="s">
-        <v>7174</v>
+        <v>7172</v>
       </c>
       <c r="F994" s="1" t="s">
-        <v>7022</v>
+        <v>7021</v>
       </c>
       <c r="G994" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45074,10 +45094,10 @@
         <v>2392</v>
       </c>
       <c r="E995" s="7" t="s">
-        <v>7175</v>
+        <v>7173</v>
       </c>
       <c r="F995" s="1" t="s">
-        <v>7023</v>
+        <v>7022</v>
       </c>
       <c r="G995" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45098,10 +45118,10 @@
         <v>2394</v>
       </c>
       <c r="E996" s="7" t="s">
-        <v>7176</v>
+        <v>7174</v>
       </c>
       <c r="F996" s="1" t="s">
-        <v>7024</v>
+        <v>7023</v>
       </c>
       <c r="G996" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45122,10 +45142,10 @@
         <v>2396</v>
       </c>
       <c r="E997" s="7" t="s">
-        <v>7177</v>
+        <v>7175</v>
       </c>
       <c r="F997" s="1" t="s">
-        <v>7025</v>
+        <v>7024</v>
       </c>
       <c r="G997" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45146,10 +45166,10 @@
         <v>2398</v>
       </c>
       <c r="E998" s="7" t="s">
-        <v>7178</v>
+        <v>7176</v>
       </c>
       <c r="F998" s="1" t="s">
-        <v>7026</v>
+        <v>7025</v>
       </c>
       <c r="G998" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45170,10 +45190,10 @@
         <v>1353</v>
       </c>
       <c r="E999" s="7" t="s">
-        <v>7179</v>
+        <v>7177</v>
       </c>
       <c r="F999" s="1" t="s">
-        <v>7027</v>
+        <v>7026</v>
       </c>
       <c r="G999" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45194,10 +45214,10 @@
         <v>2401</v>
       </c>
       <c r="E1000" s="7" t="s">
-        <v>7180</v>
+        <v>7178</v>
       </c>
       <c r="F1000" s="1" t="s">
-        <v>7028</v>
+        <v>7027</v>
       </c>
       <c r="G1000" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45218,10 +45238,10 @@
         <v>2403</v>
       </c>
       <c r="E1001" s="7" t="s">
-        <v>7181</v>
+        <v>7179</v>
       </c>
       <c r="F1001" s="1" t="s">
-        <v>7029</v>
+        <v>7028</v>
       </c>
       <c r="G1001" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45242,10 +45262,10 @@
         <v>2405</v>
       </c>
       <c r="E1002" s="7" t="s">
-        <v>7030</v>
+        <v>7029</v>
       </c>
       <c r="F1002" s="1" t="s">
-        <v>7030</v>
+        <v>7029</v>
       </c>
       <c r="G1002" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45266,10 +45286,10 @@
         <v>2407</v>
       </c>
       <c r="E1003" s="7" t="s">
-        <v>7182</v>
+        <v>7180</v>
       </c>
       <c r="F1003" s="1" t="s">
-        <v>7031</v>
+        <v>7030</v>
       </c>
       <c r="G1003" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45290,10 +45310,10 @@
         <v>2409</v>
       </c>
       <c r="E1004" s="7" t="s">
-        <v>7182</v>
+        <v>7180</v>
       </c>
       <c r="F1004" s="1" t="s">
-        <v>7031</v>
+        <v>7030</v>
       </c>
       <c r="G1004" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45314,10 +45334,10 @@
         <v>2411</v>
       </c>
       <c r="E1005" s="7" t="s">
-        <v>7183</v>
+        <v>7181</v>
       </c>
       <c r="F1005" s="1" t="s">
-        <v>7032</v>
+        <v>7031</v>
       </c>
       <c r="G1005" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45338,10 +45358,10 @@
         <v>2413</v>
       </c>
       <c r="E1006" s="7" t="s">
-        <v>7184</v>
+        <v>7182</v>
       </c>
       <c r="F1006" s="1" t="s">
-        <v>7033</v>
+        <v>7032</v>
       </c>
       <c r="G1006" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45362,10 +45382,10 @@
         <v>2415</v>
       </c>
       <c r="E1007" s="7" t="s">
-        <v>7185</v>
+        <v>7183</v>
       </c>
       <c r="F1007" s="1" t="s">
-        <v>7034</v>
+        <v>7033</v>
       </c>
       <c r="G1007" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45386,10 +45406,10 @@
         <v>2417</v>
       </c>
       <c r="E1008" s="7" t="s">
-        <v>7186</v>
+        <v>7184</v>
       </c>
       <c r="F1008" s="1" t="s">
-        <v>7035</v>
+        <v>7034</v>
       </c>
       <c r="G1008" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45410,10 +45430,10 @@
         <v>2419</v>
       </c>
       <c r="E1009" s="7" t="s">
-        <v>7187</v>
+        <v>7185</v>
       </c>
       <c r="F1009" s="1" t="s">
-        <v>7036</v>
+        <v>7035</v>
       </c>
       <c r="G1009" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45434,10 +45454,10 @@
         <v>2398</v>
       </c>
       <c r="E1010" s="7" t="s">
-        <v>7175</v>
+        <v>7173</v>
       </c>
       <c r="F1010" s="1" t="s">
-        <v>7023</v>
+        <v>7022</v>
       </c>
       <c r="G1010" s="1" t="str">
         <f t="shared" si="18"/>
@@ -45458,10 +45478,10 @@
         <v>2422</v>
       </c>
       <c r="E1011" s="7" t="s">
-        <v>7188</v>
+        <v>7186</v>
       </c>
       <c r="F1011" s="1" t="s">
-        <v>7037</v>
+        <v>7036</v>
       </c>
       <c r="G1011" s="1" t="str">
         <f t="shared" si="18"/>

</xml_diff>